<commit_message>
fixed signatures in exported officer grade list
</commit_message>
<xml_diff>
--- a/templates/список_оценок_контрактники.xlsx
+++ b/templates/список_оценок_контрактники.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="2460" windowWidth="13710" windowHeight="5085" tabRatio="920"/>
+    <workbookView xWindow="1650" yWindow="2460" windowWidth="13710" windowHeight="5085" tabRatio="920" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Главная" sheetId="2" r:id="rId1"/>
@@ -182,17 +182,17 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Огнедышащий воробей - Личное представление" guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="548" tabRatio="919" activeSheetId="8"/>
+    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
+    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
+    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
     <customWorkbookView name="Admin - Личное представление" guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="767" tabRatio="919" activeSheetId="2"/>
-    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
-    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
-    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
-    <customWorkbookView name="Огнедышащий воробей - Личное представление" guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="548" tabRatio="919" activeSheetId="8"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="74">
   <si>
     <t>№</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>год:</t>
+  </si>
+  <si>
+    <t>ЗАМЕСТИТЕЛЬ КОМАНДИРА ВОЙСКОВОЙ ЧАСТИ 74400 - НАЧАЛЬНИК УЧЕБНОГО ОТДЕЛЕНИЯ</t>
+  </si>
+  <si>
+    <t>подполковник</t>
+  </si>
+  <si>
+    <t>А. Федосеев</t>
   </si>
 </sst>
 </file>
@@ -1616,6 +1625,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -1638,18 +1650,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1684,6 +1684,18 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1709,9 +1721,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2103,8 +2112,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J3"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2158,12 +2167,12 @@
       <c r="D3" s="192"/>
       <c r="E3" s="192"/>
       <c r="F3" s="193"/>
-      <c r="G3" s="218">
+      <c r="G3" s="194">
         <v>2014</v>
       </c>
-      <c r="H3" s="218"/>
-      <c r="I3" s="218"/>
-      <c r="J3" s="218"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="126"/>
@@ -2179,17 +2188,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="85" showPageBreaks="1" printArea="1">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="85" showPageBreaks="1" printArea="1">
       <pane xSplit="30" ySplit="28" topLeftCell="AE29" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="85" showPageBreaks="1" printArea="1">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="85" showPageBreaks="1" printArea="1">
       <pane xSplit="30" ySplit="28" topLeftCell="AE29" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2219,10 +2228,10 @@
   </sheetPr>
   <dimension ref="B1:Z342"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:Y3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2314,62 +2323,62 @@
       <c r="Z1" s="124"/>
     </row>
     <row r="2" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="197"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="197"/>
-      <c r="W2" s="197"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="198"/>
+      <c r="W2" s="198"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
       <c r="Z2" s="124"/>
     </row>
     <row r="3" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="197"/>
-      <c r="O3" s="197"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="197"/>
-      <c r="R3" s="197"/>
-      <c r="S3" s="197"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="197"/>
-      <c r="V3" s="197"/>
-      <c r="W3" s="197"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="198"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="198"/>
+      <c r="Q3" s="198"/>
+      <c r="R3" s="198"/>
+      <c r="S3" s="198"/>
+      <c r="T3" s="198"/>
+      <c r="U3" s="198"/>
+      <c r="V3" s="198"/>
+      <c r="W3" s="198"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
       <c r="Z3" s="124"/>
     </row>
     <row r="4" spans="2:26" s="110" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -2500,117 +2509,114 @@
       <c r="Y6" s="180"/>
     </row>
     <row r="7" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="195"/>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195"/>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="195"/>
-      <c r="I7" s="195"/>
-      <c r="J7" s="195"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="195"/>
-      <c r="M7" s="195"/>
-      <c r="N7" s="195"/>
-      <c r="O7" s="195"/>
-      <c r="P7" s="195"/>
-      <c r="Q7" s="195"/>
-      <c r="R7" s="195"/>
-      <c r="S7" s="195"/>
-      <c r="T7" s="195"/>
-      <c r="U7" s="195"/>
-      <c r="V7" s="195"/>
-      <c r="W7" s="195"/>
-      <c r="X7" s="195"/>
-      <c r="Y7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="196"/>
+      <c r="E7" s="196"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="196"/>
+      <c r="H7" s="196"/>
+      <c r="I7" s="196"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="196"/>
+      <c r="N7" s="196"/>
+      <c r="O7" s="196"/>
+      <c r="P7" s="196"/>
+      <c r="Q7" s="196"/>
+      <c r="R7" s="196"/>
+      <c r="S7" s="196"/>
+      <c r="T7" s="196"/>
+      <c r="U7" s="196"/>
+      <c r="V7" s="196"/>
+      <c r="W7" s="196"/>
+      <c r="X7" s="196"/>
+      <c r="Y7" s="196"/>
     </row>
     <row r="8" spans="2:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C8" s="198"/>
-      <c r="D8" s="198"/>
-      <c r="E8" s="198"/>
-      <c r="F8" s="198"/>
-      <c r="G8" s="198"/>
-      <c r="H8" s="198"/>
-      <c r="I8" s="198"/>
-      <c r="J8" s="198"/>
-      <c r="K8" s="198"/>
-      <c r="L8" s="198"/>
-      <c r="M8" s="198"/>
-      <c r="N8" s="198"/>
-      <c r="O8" s="198"/>
-      <c r="P8" s="198"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="198"/>
-      <c r="S8" s="198"/>
-      <c r="T8" s="198"/>
-      <c r="U8" s="198"/>
-      <c r="V8" s="198"/>
-      <c r="W8" s="198"/>
-      <c r="X8" s="198"/>
-      <c r="Y8" s="198"/>
+      <c r="B8" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="199"/>
+      <c r="D8" s="199"/>
+      <c r="E8" s="199"/>
+      <c r="F8" s="199"/>
+      <c r="G8" s="199"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="199"/>
+      <c r="L8" s="199"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="199"/>
+      <c r="R8" s="199"/>
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="199"/>
+      <c r="W8" s="199"/>
+      <c r="X8" s="199"/>
+      <c r="Y8" s="199"/>
     </row>
     <row r="9" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="199"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="199"/>
-      <c r="H9" s="199"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="199"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="199"/>
-      <c r="M9" s="199"/>
-      <c r="N9" s="199"/>
-      <c r="O9" s="199"/>
-      <c r="P9" s="199"/>
-      <c r="Q9" s="199"/>
-      <c r="R9" s="199"/>
-      <c r="S9" s="199"/>
-      <c r="T9" s="199"/>
-      <c r="U9" s="199"/>
-      <c r="V9" s="199"/>
-      <c r="W9" s="199"/>
-      <c r="X9" s="199"/>
-      <c r="Y9" s="199"/>
+      <c r="B9" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="200"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
+      <c r="L9" s="200"/>
+      <c r="M9" s="200"/>
+      <c r="N9" s="200"/>
+      <c r="O9" s="200"/>
+      <c r="P9" s="200"/>
+      <c r="Q9" s="200"/>
+      <c r="R9" s="200"/>
+      <c r="S9" s="200"/>
+      <c r="T9" s="200"/>
+      <c r="U9" s="200"/>
+      <c r="V9" s="200"/>
+      <c r="W9" s="200"/>
+      <c r="X9" s="200"/>
+      <c r="Y9" s="200"/>
     </row>
     <row r="10" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C10" s="194"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="194"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="194"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="194"/>
-      <c r="M10" s="194"/>
-      <c r="N10" s="194"/>
-      <c r="O10" s="194"/>
-      <c r="P10" s="194"/>
-      <c r="Q10" s="194"/>
-      <c r="R10" s="194"/>
-      <c r="S10" s="194"/>
-      <c r="T10" s="194"/>
-      <c r="U10" s="194"/>
-      <c r="V10" s="194"/>
-      <c r="W10" s="194"/>
-      <c r="X10" s="194"/>
-      <c r="Y10" s="194"/>
+      <c r="B10" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="195"/>
+      <c r="I10" s="195"/>
+      <c r="J10" s="195"/>
+      <c r="K10" s="195"/>
+      <c r="L10" s="195"/>
+      <c r="M10" s="195"/>
+      <c r="N10" s="195"/>
+      <c r="O10" s="195"/>
+      <c r="P10" s="195"/>
+      <c r="Q10" s="195"/>
+      <c r="R10" s="195"/>
+      <c r="S10" s="195"/>
+      <c r="T10" s="195"/>
+      <c r="U10" s="195"/>
+      <c r="V10" s="195"/>
+      <c r="W10" s="195"/>
+      <c r="X10" s="195"/>
+      <c r="Y10" s="195"/>
     </row>
     <row r="342" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B342" s="148"/>
@@ -2663,10 +2669,10 @@
   </sheetPr>
   <dimension ref="A1:Y971"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30:Y30"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34:Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2756,89 +2762,89 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="1:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="196"/>
-      <c r="S3" s="196"/>
-      <c r="T3" s="196"/>
-      <c r="U3" s="196"/>
-      <c r="V3" s="196"/>
-      <c r="W3" s="196"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="197"/>
+      <c r="Q3" s="197"/>
+      <c r="R3" s="197"/>
+      <c r="S3" s="197"/>
+      <c r="T3" s="197"/>
+      <c r="U3" s="197"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="197"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="1:25" s="110" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="206" t="s">
+      <c r="B4" s="204" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="207"/>
-      <c r="G4" s="207"/>
-      <c r="H4" s="207"/>
-      <c r="I4" s="207"/>
-      <c r="J4" s="207"/>
-      <c r="K4" s="207"/>
-      <c r="L4" s="207"/>
-      <c r="M4" s="207"/>
-      <c r="N4" s="207"/>
-      <c r="O4" s="207"/>
-      <c r="P4" s="207"/>
-      <c r="Q4" s="207"/>
-      <c r="R4" s="207"/>
-      <c r="S4" s="207"/>
-      <c r="T4" s="207"/>
-      <c r="U4" s="207"/>
-      <c r="V4" s="207"/>
-      <c r="W4" s="207"/>
-      <c r="X4" s="207"/>
-      <c r="Y4" s="208"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="205"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="205"/>
+      <c r="J4" s="205"/>
+      <c r="K4" s="205"/>
+      <c r="L4" s="205"/>
+      <c r="M4" s="205"/>
+      <c r="N4" s="205"/>
+      <c r="O4" s="205"/>
+      <c r="P4" s="205"/>
+      <c r="Q4" s="205"/>
+      <c r="R4" s="205"/>
+      <c r="S4" s="205"/>
+      <c r="T4" s="205"/>
+      <c r="U4" s="205"/>
+      <c r="V4" s="205"/>
+      <c r="W4" s="205"/>
+      <c r="X4" s="205"/>
+      <c r="Y4" s="206"/>
     </row>
     <row r="5" spans="1:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="137"/>
@@ -2972,32 +2978,32 @@
       <c r="X8" s="116"/>
     </row>
     <row r="9" spans="1:25" s="110" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="206" t="s">
+      <c r="B9" s="204" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="207"/>
-      <c r="D9" s="207"/>
-      <c r="E9" s="207"/>
-      <c r="F9" s="207"/>
-      <c r="G9" s="207"/>
-      <c r="H9" s="207"/>
-      <c r="I9" s="207"/>
-      <c r="J9" s="207"/>
-      <c r="K9" s="207"/>
-      <c r="L9" s="207"/>
-      <c r="M9" s="207"/>
-      <c r="N9" s="207"/>
-      <c r="O9" s="207"/>
-      <c r="P9" s="207"/>
-      <c r="Q9" s="207"/>
-      <c r="R9" s="207"/>
-      <c r="S9" s="207"/>
-      <c r="T9" s="207"/>
-      <c r="U9" s="207"/>
-      <c r="V9" s="207"/>
-      <c r="W9" s="207"/>
-      <c r="X9" s="207"/>
-      <c r="Y9" s="208"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="205"/>
+      <c r="K9" s="205"/>
+      <c r="L9" s="205"/>
+      <c r="M9" s="205"/>
+      <c r="N9" s="205"/>
+      <c r="O9" s="205"/>
+      <c r="P9" s="205"/>
+      <c r="Q9" s="205"/>
+      <c r="R9" s="205"/>
+      <c r="S9" s="205"/>
+      <c r="T9" s="205"/>
+      <c r="U9" s="205"/>
+      <c r="V9" s="205"/>
+      <c r="W9" s="205"/>
+      <c r="X9" s="205"/>
+      <c r="Y9" s="206"/>
     </row>
     <row r="10" spans="1:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="141" t="s">
@@ -3130,32 +3136,32 @@
       <c r="X13" s="116"/>
     </row>
     <row r="14" spans="1:25" s="110" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="206" t="s">
+      <c r="B14" s="204" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="207"/>
-      <c r="D14" s="207"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="207"/>
-      <c r="G14" s="207"/>
-      <c r="H14" s="207"/>
-      <c r="I14" s="207"/>
-      <c r="J14" s="207"/>
-      <c r="K14" s="207"/>
-      <c r="L14" s="207"/>
-      <c r="M14" s="207"/>
-      <c r="N14" s="207"/>
-      <c r="O14" s="207"/>
-      <c r="P14" s="207"/>
-      <c r="Q14" s="207"/>
-      <c r="R14" s="207"/>
-      <c r="S14" s="207"/>
-      <c r="T14" s="207"/>
-      <c r="U14" s="207"/>
-      <c r="V14" s="207"/>
-      <c r="W14" s="207"/>
-      <c r="X14" s="207"/>
-      <c r="Y14" s="208"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="205"/>
+      <c r="I14" s="205"/>
+      <c r="J14" s="205"/>
+      <c r="K14" s="205"/>
+      <c r="L14" s="205"/>
+      <c r="M14" s="205"/>
+      <c r="N14" s="205"/>
+      <c r="O14" s="205"/>
+      <c r="P14" s="205"/>
+      <c r="Q14" s="205"/>
+      <c r="R14" s="205"/>
+      <c r="S14" s="205"/>
+      <c r="T14" s="205"/>
+      <c r="U14" s="205"/>
+      <c r="V14" s="205"/>
+      <c r="W14" s="205"/>
+      <c r="X14" s="205"/>
+      <c r="Y14" s="206"/>
     </row>
     <row r="15" spans="1:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
@@ -3308,32 +3314,32 @@
       <c r="X18" s="118"/>
     </row>
     <row r="19" spans="2:25" s="110" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="206" t="s">
+      <c r="B19" s="204" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="207"/>
-      <c r="D19" s="207"/>
-      <c r="E19" s="204"/>
-      <c r="F19" s="207"/>
-      <c r="G19" s="207"/>
-      <c r="H19" s="207"/>
-      <c r="I19" s="207"/>
-      <c r="J19" s="207"/>
-      <c r="K19" s="207"/>
-      <c r="L19" s="207"/>
-      <c r="M19" s="207"/>
-      <c r="N19" s="207"/>
-      <c r="O19" s="207"/>
-      <c r="P19" s="207"/>
-      <c r="Q19" s="207"/>
-      <c r="R19" s="207"/>
-      <c r="S19" s="207"/>
-      <c r="T19" s="207"/>
-      <c r="U19" s="207"/>
-      <c r="V19" s="207"/>
-      <c r="W19" s="207"/>
-      <c r="X19" s="207"/>
-      <c r="Y19" s="208"/>
+      <c r="C19" s="205"/>
+      <c r="D19" s="205"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
+      <c r="K19" s="205"/>
+      <c r="L19" s="205"/>
+      <c r="M19" s="205"/>
+      <c r="N19" s="205"/>
+      <c r="O19" s="205"/>
+      <c r="P19" s="205"/>
+      <c r="Q19" s="205"/>
+      <c r="R19" s="205"/>
+      <c r="S19" s="205"/>
+      <c r="T19" s="205"/>
+      <c r="U19" s="205"/>
+      <c r="V19" s="205"/>
+      <c r="W19" s="205"/>
+      <c r="X19" s="205"/>
+      <c r="Y19" s="206"/>
     </row>
     <row r="20" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="141" t="s">
@@ -3462,58 +3468,58 @@
       <c r="Y22" s="117"/>
     </row>
     <row r="23" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="209"/>
-      <c r="C23" s="209"/>
-      <c r="D23" s="209"/>
-      <c r="E23" s="210"/>
-      <c r="F23" s="209"/>
-      <c r="G23" s="209"/>
-      <c r="H23" s="209"/>
-      <c r="I23" s="209"/>
-      <c r="J23" s="209"/>
-      <c r="K23" s="209"/>
-      <c r="L23" s="209"/>
-      <c r="M23" s="209"/>
-      <c r="N23" s="209"/>
-      <c r="O23" s="209"/>
-      <c r="P23" s="209"/>
-      <c r="Q23" s="209"/>
-      <c r="R23" s="209"/>
-      <c r="S23" s="209"/>
-      <c r="T23" s="209"/>
-      <c r="U23" s="209"/>
-      <c r="V23" s="209"/>
-      <c r="W23" s="209"/>
-      <c r="X23" s="209"/>
-      <c r="Y23" s="209"/>
+      <c r="B23" s="207"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="207"/>
+      <c r="E23" s="208"/>
+      <c r="F23" s="207"/>
+      <c r="G23" s="207"/>
+      <c r="H23" s="207"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="207"/>
+      <c r="K23" s="207"/>
+      <c r="L23" s="207"/>
+      <c r="M23" s="207"/>
+      <c r="N23" s="207"/>
+      <c r="O23" s="207"/>
+      <c r="P23" s="207"/>
+      <c r="Q23" s="207"/>
+      <c r="R23" s="207"/>
+      <c r="S23" s="207"/>
+      <c r="T23" s="207"/>
+      <c r="U23" s="207"/>
+      <c r="V23" s="207"/>
+      <c r="W23" s="207"/>
+      <c r="X23" s="207"/>
+      <c r="Y23" s="207"/>
     </row>
     <row r="24" spans="2:25" s="110" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="203" t="s">
+      <c r="B24" s="201" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="204"/>
-      <c r="D24" s="204"/>
-      <c r="E24" s="204"/>
-      <c r="F24" s="204"/>
-      <c r="G24" s="204"/>
-      <c r="H24" s="204"/>
-      <c r="I24" s="204"/>
-      <c r="J24" s="204"/>
-      <c r="K24" s="204"/>
-      <c r="L24" s="204"/>
-      <c r="M24" s="204"/>
-      <c r="N24" s="204"/>
-      <c r="O24" s="204"/>
-      <c r="P24" s="204"/>
-      <c r="Q24" s="204"/>
-      <c r="R24" s="204"/>
-      <c r="S24" s="204"/>
-      <c r="T24" s="204"/>
-      <c r="U24" s="204"/>
-      <c r="V24" s="204"/>
-      <c r="W24" s="204"/>
-      <c r="X24" s="204"/>
-      <c r="Y24" s="205"/>
+      <c r="C24" s="202"/>
+      <c r="D24" s="202"/>
+      <c r="E24" s="202"/>
+      <c r="F24" s="202"/>
+      <c r="G24" s="202"/>
+      <c r="H24" s="202"/>
+      <c r="I24" s="202"/>
+      <c r="J24" s="202"/>
+      <c r="K24" s="202"/>
+      <c r="L24" s="202"/>
+      <c r="M24" s="202"/>
+      <c r="N24" s="202"/>
+      <c r="O24" s="202"/>
+      <c r="P24" s="202"/>
+      <c r="Q24" s="202"/>
+      <c r="R24" s="202"/>
+      <c r="S24" s="202"/>
+      <c r="T24" s="202"/>
+      <c r="U24" s="202"/>
+      <c r="V24" s="202"/>
+      <c r="W24" s="202"/>
+      <c r="X24" s="202"/>
+      <c r="Y24" s="203"/>
     </row>
     <row r="25" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="141" t="s">
@@ -3666,32 +3672,32 @@
       <c r="X28" s="118"/>
     </row>
     <row r="29" spans="2:25" s="110" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="200" t="s">
+      <c r="B29" s="209" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="201"/>
-      <c r="D29" s="201"/>
-      <c r="E29" s="201"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="201"/>
-      <c r="H29" s="201"/>
-      <c r="I29" s="201"/>
-      <c r="J29" s="201"/>
-      <c r="K29" s="201"/>
-      <c r="L29" s="201"/>
-      <c r="M29" s="201"/>
-      <c r="N29" s="201"/>
-      <c r="O29" s="201"/>
-      <c r="P29" s="201"/>
-      <c r="Q29" s="201"/>
-      <c r="R29" s="201"/>
-      <c r="S29" s="201"/>
-      <c r="T29" s="201"/>
-      <c r="U29" s="201"/>
-      <c r="V29" s="201"/>
-      <c r="W29" s="201"/>
-      <c r="X29" s="201"/>
-      <c r="Y29" s="202"/>
+      <c r="C29" s="210"/>
+      <c r="D29" s="210"/>
+      <c r="E29" s="210"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="210"/>
+      <c r="H29" s="210"/>
+      <c r="I29" s="210"/>
+      <c r="J29" s="210"/>
+      <c r="K29" s="210"/>
+      <c r="L29" s="210"/>
+      <c r="M29" s="210"/>
+      <c r="N29" s="210"/>
+      <c r="O29" s="210"/>
+      <c r="P29" s="210"/>
+      <c r="Q29" s="210"/>
+      <c r="R29" s="210"/>
+      <c r="S29" s="210"/>
+      <c r="T29" s="210"/>
+      <c r="U29" s="210"/>
+      <c r="V29" s="210"/>
+      <c r="W29" s="210"/>
+      <c r="X29" s="210"/>
+      <c r="Y29" s="211"/>
     </row>
     <row r="30" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="141" t="s">
@@ -3820,117 +3826,114 @@
       <c r="Y32" s="117"/>
     </row>
     <row r="33" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="195"/>
-      <c r="C33" s="195"/>
-      <c r="D33" s="195"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
-      <c r="K33" s="195"/>
-      <c r="L33" s="195"/>
-      <c r="M33" s="195"/>
-      <c r="N33" s="195"/>
-      <c r="O33" s="195"/>
-      <c r="P33" s="195"/>
-      <c r="Q33" s="195"/>
-      <c r="R33" s="195"/>
-      <c r="S33" s="195"/>
-      <c r="T33" s="195"/>
-      <c r="U33" s="195"/>
-      <c r="V33" s="195"/>
-      <c r="W33" s="195"/>
-      <c r="X33" s="195"/>
-      <c r="Y33" s="195"/>
-    </row>
-    <row r="34" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C34" s="198"/>
-      <c r="D34" s="198"/>
-      <c r="E34" s="198"/>
-      <c r="F34" s="198"/>
-      <c r="G34" s="198"/>
-      <c r="H34" s="198"/>
-      <c r="I34" s="198"/>
-      <c r="J34" s="198"/>
-      <c r="K34" s="198"/>
-      <c r="L34" s="198"/>
-      <c r="M34" s="198"/>
-      <c r="N34" s="198"/>
-      <c r="O34" s="198"/>
-      <c r="P34" s="198"/>
-      <c r="Q34" s="198"/>
-      <c r="R34" s="198"/>
-      <c r="S34" s="198"/>
-      <c r="T34" s="198"/>
-      <c r="U34" s="198"/>
-      <c r="V34" s="198"/>
-      <c r="W34" s="198"/>
-      <c r="X34" s="198"/>
-      <c r="Y34" s="198"/>
+      <c r="B33" s="196"/>
+      <c r="C33" s="196"/>
+      <c r="D33" s="196"/>
+      <c r="E33" s="196"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="196"/>
+      <c r="H33" s="196"/>
+      <c r="I33" s="196"/>
+      <c r="J33" s="196"/>
+      <c r="K33" s="196"/>
+      <c r="L33" s="196"/>
+      <c r="M33" s="196"/>
+      <c r="N33" s="196"/>
+      <c r="O33" s="196"/>
+      <c r="P33" s="196"/>
+      <c r="Q33" s="196"/>
+      <c r="R33" s="196"/>
+      <c r="S33" s="196"/>
+      <c r="T33" s="196"/>
+      <c r="U33" s="196"/>
+      <c r="V33" s="196"/>
+      <c r="W33" s="196"/>
+      <c r="X33" s="196"/>
+      <c r="Y33" s="196"/>
+    </row>
+    <row r="34" spans="2:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="199"/>
+      <c r="D34" s="199"/>
+      <c r="E34" s="199"/>
+      <c r="F34" s="199"/>
+      <c r="G34" s="199"/>
+      <c r="H34" s="199"/>
+      <c r="I34" s="199"/>
+      <c r="J34" s="199"/>
+      <c r="K34" s="199"/>
+      <c r="L34" s="199"/>
+      <c r="M34" s="199"/>
+      <c r="N34" s="199"/>
+      <c r="O34" s="199"/>
+      <c r="P34" s="199"/>
+      <c r="Q34" s="199"/>
+      <c r="R34" s="199"/>
+      <c r="S34" s="199"/>
+      <c r="T34" s="199"/>
+      <c r="U34" s="199"/>
+      <c r="V34" s="199"/>
+      <c r="W34" s="199"/>
+      <c r="X34" s="199"/>
+      <c r="Y34" s="199"/>
     </row>
     <row r="35" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C35" s="199"/>
-      <c r="D35" s="199"/>
-      <c r="E35" s="199"/>
-      <c r="F35" s="199"/>
-      <c r="G35" s="199"/>
-      <c r="H35" s="199"/>
-      <c r="I35" s="199"/>
-      <c r="J35" s="199"/>
-      <c r="K35" s="199"/>
-      <c r="L35" s="199"/>
-      <c r="M35" s="199"/>
-      <c r="N35" s="199"/>
-      <c r="O35" s="199"/>
-      <c r="P35" s="199"/>
-      <c r="Q35" s="199"/>
-      <c r="R35" s="199"/>
-      <c r="S35" s="199"/>
-      <c r="T35" s="199"/>
-      <c r="U35" s="199"/>
-      <c r="V35" s="199"/>
-      <c r="W35" s="199"/>
-      <c r="X35" s="199"/>
-      <c r="Y35" s="199"/>
+      <c r="B35" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="200"/>
+      <c r="D35" s="200"/>
+      <c r="E35" s="200"/>
+      <c r="F35" s="200"/>
+      <c r="G35" s="200"/>
+      <c r="H35" s="200"/>
+      <c r="I35" s="200"/>
+      <c r="J35" s="200"/>
+      <c r="K35" s="200"/>
+      <c r="L35" s="200"/>
+      <c r="M35" s="200"/>
+      <c r="N35" s="200"/>
+      <c r="O35" s="200"/>
+      <c r="P35" s="200"/>
+      <c r="Q35" s="200"/>
+      <c r="R35" s="200"/>
+      <c r="S35" s="200"/>
+      <c r="T35" s="200"/>
+      <c r="U35" s="200"/>
+      <c r="V35" s="200"/>
+      <c r="W35" s="200"/>
+      <c r="X35" s="200"/>
+      <c r="Y35" s="200"/>
     </row>
     <row r="36" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C36" s="194"/>
-      <c r="D36" s="194"/>
-      <c r="E36" s="194"/>
-      <c r="F36" s="194"/>
-      <c r="G36" s="194"/>
-      <c r="H36" s="194"/>
-      <c r="I36" s="194"/>
-      <c r="J36" s="194"/>
-      <c r="K36" s="194"/>
-      <c r="L36" s="194"/>
-      <c r="M36" s="194"/>
-      <c r="N36" s="194"/>
-      <c r="O36" s="194"/>
-      <c r="P36" s="194"/>
-      <c r="Q36" s="194"/>
-      <c r="R36" s="194"/>
-      <c r="S36" s="194"/>
-      <c r="T36" s="194"/>
-      <c r="U36" s="194"/>
-      <c r="V36" s="194"/>
-      <c r="W36" s="194"/>
-      <c r="X36" s="194"/>
-      <c r="Y36" s="194"/>
+      <c r="B36" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="195"/>
+      <c r="D36" s="195"/>
+      <c r="E36" s="195"/>
+      <c r="F36" s="195"/>
+      <c r="G36" s="195"/>
+      <c r="H36" s="195"/>
+      <c r="I36" s="195"/>
+      <c r="J36" s="195"/>
+      <c r="K36" s="195"/>
+      <c r="L36" s="195"/>
+      <c r="M36" s="195"/>
+      <c r="N36" s="195"/>
+      <c r="O36" s="195"/>
+      <c r="P36" s="195"/>
+      <c r="Q36" s="195"/>
+      <c r="R36" s="195"/>
+      <c r="S36" s="195"/>
+      <c r="T36" s="195"/>
+      <c r="U36" s="195"/>
+      <c r="V36" s="195"/>
+      <c r="W36" s="195"/>
+      <c r="X36" s="195"/>
+      <c r="Y36" s="195"/>
     </row>
     <row r="289" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B289" s="148"/>
@@ -3997,6 +4000,11 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="13">
+    <mergeCell ref="B36:Y36"/>
+    <mergeCell ref="B35:Y35"/>
+    <mergeCell ref="B34:Y34"/>
+    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="B29:Y29"/>
     <mergeCell ref="B24:Y24"/>
     <mergeCell ref="B3:Y3"/>
     <mergeCell ref="B4:Y4"/>
@@ -4005,11 +4013,6 @@
     <mergeCell ref="B23:Y23"/>
     <mergeCell ref="B14:Y14"/>
     <mergeCell ref="B19:Y19"/>
-    <mergeCell ref="B36:Y36"/>
-    <mergeCell ref="B35:Y35"/>
-    <mergeCell ref="B34:Y34"/>
-    <mergeCell ref="B33:Y33"/>
-    <mergeCell ref="B29:Y29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.69" bottom="0.27" header="0.84" footer="0.28999999999999998"/>
@@ -4032,7 +4035,7 @@
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:Y20"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4122,89 +4125,89 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="197"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="197"/>
-      <c r="W2" s="197"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="198"/>
+      <c r="W2" s="198"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="197"/>
-      <c r="O3" s="197"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="197"/>
-      <c r="R3" s="197"/>
-      <c r="S3" s="197"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="197"/>
-      <c r="V3" s="197"/>
-      <c r="W3" s="197"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="198"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="198"/>
+      <c r="Q3" s="198"/>
+      <c r="R3" s="198"/>
+      <c r="S3" s="198"/>
+      <c r="T3" s="198"/>
+      <c r="U3" s="198"/>
+      <c r="V3" s="198"/>
+      <c r="W3" s="198"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="201" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
-      <c r="L4" s="204"/>
-      <c r="M4" s="204"/>
-      <c r="N4" s="204"/>
-      <c r="O4" s="204"/>
-      <c r="P4" s="204"/>
-      <c r="Q4" s="204"/>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="204"/>
-      <c r="X4" s="204"/>
-      <c r="Y4" s="205"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="202"/>
+      <c r="S4" s="202"/>
+      <c r="T4" s="202"/>
+      <c r="U4" s="202"/>
+      <c r="V4" s="202"/>
+      <c r="W4" s="202"/>
+      <c r="X4" s="202"/>
+      <c r="Y4" s="203"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -4359,32 +4362,32 @@
       <c r="Y8" s="156"/>
     </row>
     <row r="9" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="201" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="204"/>
-      <c r="D9" s="204"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="204"/>
-      <c r="H9" s="204"/>
-      <c r="I9" s="204"/>
-      <c r="J9" s="204"/>
-      <c r="K9" s="204"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="204"/>
-      <c r="N9" s="204"/>
-      <c r="O9" s="204"/>
-      <c r="P9" s="204"/>
-      <c r="Q9" s="204"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="204"/>
-      <c r="U9" s="204"/>
-      <c r="V9" s="204"/>
-      <c r="W9" s="204"/>
-      <c r="X9" s="204"/>
-      <c r="Y9" s="205"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="202"/>
+      <c r="J9" s="202"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="202"/>
+      <c r="S9" s="202"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="202"/>
+      <c r="X9" s="202"/>
+      <c r="Y9" s="203"/>
     </row>
     <row r="10" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="141" t="s">
@@ -4539,32 +4542,32 @@
       <c r="Y13" s="159"/>
     </row>
     <row r="14" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="203" t="s">
+      <c r="B14" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="204"/>
-      <c r="D14" s="204"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="204"/>
-      <c r="G14" s="204"/>
-      <c r="H14" s="204"/>
-      <c r="I14" s="204"/>
-      <c r="J14" s="204"/>
-      <c r="K14" s="204"/>
-      <c r="L14" s="204"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="204"/>
-      <c r="O14" s="204"/>
-      <c r="P14" s="204"/>
-      <c r="Q14" s="204"/>
-      <c r="R14" s="204"/>
-      <c r="S14" s="204"/>
-      <c r="T14" s="204"/>
-      <c r="U14" s="204"/>
-      <c r="V14" s="204"/>
-      <c r="W14" s="204"/>
-      <c r="X14" s="204"/>
-      <c r="Y14" s="205"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="202"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+      <c r="Q14" s="202"/>
+      <c r="R14" s="202"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
+      <c r="U14" s="202"/>
+      <c r="V14" s="202"/>
+      <c r="W14" s="202"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="203"/>
     </row>
     <row r="15" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
@@ -4719,32 +4722,32 @@
       <c r="Y18" s="137"/>
     </row>
     <row r="19" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="203" t="s">
+      <c r="B19" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="204"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="204"/>
-      <c r="F19" s="204"/>
-      <c r="G19" s="204"/>
-      <c r="H19" s="204"/>
-      <c r="I19" s="204"/>
-      <c r="J19" s="204"/>
-      <c r="K19" s="204"/>
-      <c r="L19" s="204"/>
-      <c r="M19" s="204"/>
-      <c r="N19" s="204"/>
-      <c r="O19" s="204"/>
-      <c r="P19" s="204"/>
-      <c r="Q19" s="204"/>
-      <c r="R19" s="204"/>
-      <c r="S19" s="204"/>
-      <c r="T19" s="204"/>
-      <c r="U19" s="204"/>
-      <c r="V19" s="204"/>
-      <c r="W19" s="204"/>
-      <c r="X19" s="204"/>
-      <c r="Y19" s="205"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="202"/>
+      <c r="M19" s="202"/>
+      <c r="N19" s="202"/>
+      <c r="O19" s="202"/>
+      <c r="P19" s="202"/>
+      <c r="Q19" s="202"/>
+      <c r="R19" s="202"/>
+      <c r="S19" s="202"/>
+      <c r="T19" s="202"/>
+      <c r="U19" s="202"/>
+      <c r="V19" s="202"/>
+      <c r="W19" s="202"/>
+      <c r="X19" s="202"/>
+      <c r="Y19" s="203"/>
     </row>
     <row r="20" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="141" t="s">
@@ -4847,117 +4850,114 @@
       <c r="Y21" s="180"/>
     </row>
     <row r="22" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="195"/>
-      <c r="C22" s="195"/>
-      <c r="D22" s="195"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="195"/>
-      <c r="L22" s="195"/>
-      <c r="M22" s="195"/>
-      <c r="N22" s="195"/>
-      <c r="O22" s="195"/>
-      <c r="P22" s="195"/>
-      <c r="Q22" s="195"/>
-      <c r="R22" s="195"/>
-      <c r="S22" s="195"/>
-      <c r="T22" s="195"/>
-      <c r="U22" s="195"/>
-      <c r="V22" s="195"/>
-      <c r="W22" s="195"/>
-      <c r="X22" s="195"/>
-      <c r="Y22" s="195"/>
+      <c r="B22" s="196"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="196"/>
+      <c r="E22" s="196"/>
+      <c r="F22" s="196"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+      <c r="K22" s="196"/>
+      <c r="L22" s="196"/>
+      <c r="M22" s="196"/>
+      <c r="N22" s="196"/>
+      <c r="O22" s="196"/>
+      <c r="P22" s="196"/>
+      <c r="Q22" s="196"/>
+      <c r="R22" s="196"/>
+      <c r="S22" s="196"/>
+      <c r="T22" s="196"/>
+      <c r="U22" s="196"/>
+      <c r="V22" s="196"/>
+      <c r="W22" s="196"/>
+      <c r="X22" s="196"/>
+      <c r="Y22" s="196"/>
     </row>
     <row r="23" spans="2:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="198"/>
-      <c r="D23" s="198"/>
-      <c r="E23" s="198"/>
-      <c r="F23" s="198"/>
-      <c r="G23" s="198"/>
-      <c r="H23" s="198"/>
-      <c r="I23" s="198"/>
-      <c r="J23" s="198"/>
-      <c r="K23" s="198"/>
-      <c r="L23" s="198"/>
-      <c r="M23" s="198"/>
-      <c r="N23" s="198"/>
-      <c r="O23" s="198"/>
-      <c r="P23" s="198"/>
-      <c r="Q23" s="198"/>
-      <c r="R23" s="198"/>
-      <c r="S23" s="198"/>
-      <c r="T23" s="198"/>
-      <c r="U23" s="198"/>
-      <c r="V23" s="198"/>
-      <c r="W23" s="198"/>
-      <c r="X23" s="198"/>
-      <c r="Y23" s="198"/>
+      <c r="B23" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="199"/>
+      <c r="D23" s="199"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
+      <c r="G23" s="199"/>
+      <c r="H23" s="199"/>
+      <c r="I23" s="199"/>
+      <c r="J23" s="199"/>
+      <c r="K23" s="199"/>
+      <c r="L23" s="199"/>
+      <c r="M23" s="199"/>
+      <c r="N23" s="199"/>
+      <c r="O23" s="199"/>
+      <c r="P23" s="199"/>
+      <c r="Q23" s="199"/>
+      <c r="R23" s="199"/>
+      <c r="S23" s="199"/>
+      <c r="T23" s="199"/>
+      <c r="U23" s="199"/>
+      <c r="V23" s="199"/>
+      <c r="W23" s="199"/>
+      <c r="X23" s="199"/>
+      <c r="Y23" s="199"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C24" s="199"/>
-      <c r="D24" s="199"/>
-      <c r="E24" s="199"/>
-      <c r="F24" s="199"/>
-      <c r="G24" s="199"/>
-      <c r="H24" s="199"/>
-      <c r="I24" s="199"/>
-      <c r="J24" s="199"/>
-      <c r="K24" s="199"/>
-      <c r="L24" s="199"/>
-      <c r="M24" s="199"/>
-      <c r="N24" s="199"/>
-      <c r="O24" s="199"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="199"/>
-      <c r="R24" s="199"/>
-      <c r="S24" s="199"/>
-      <c r="T24" s="199"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="199"/>
-      <c r="W24" s="199"/>
-      <c r="X24" s="199"/>
-      <c r="Y24" s="199"/>
+      <c r="B24" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="200"/>
+      <c r="I24" s="200"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="200"/>
+      <c r="L24" s="200"/>
+      <c r="M24" s="200"/>
+      <c r="N24" s="200"/>
+      <c r="O24" s="200"/>
+      <c r="P24" s="200"/>
+      <c r="Q24" s="200"/>
+      <c r="R24" s="200"/>
+      <c r="S24" s="200"/>
+      <c r="T24" s="200"/>
+      <c r="U24" s="200"/>
+      <c r="V24" s="200"/>
+      <c r="W24" s="200"/>
+      <c r="X24" s="200"/>
+      <c r="Y24" s="200"/>
     </row>
     <row r="25" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="194"/>
-      <c r="K25" s="194"/>
-      <c r="L25" s="194"/>
-      <c r="M25" s="194"/>
-      <c r="N25" s="194"/>
-      <c r="O25" s="194"/>
-      <c r="P25" s="194"/>
-      <c r="Q25" s="194"/>
-      <c r="R25" s="194"/>
-      <c r="S25" s="194"/>
-      <c r="T25" s="194"/>
-      <c r="U25" s="194"/>
-      <c r="V25" s="194"/>
-      <c r="W25" s="194"/>
-      <c r="X25" s="194"/>
-      <c r="Y25" s="194"/>
+      <c r="B25" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="195"/>
+      <c r="D25" s="195"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="195"/>
+      <c r="H25" s="195"/>
+      <c r="I25" s="195"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="N25" s="195"/>
+      <c r="O25" s="195"/>
+      <c r="P25" s="195"/>
+      <c r="Q25" s="195"/>
+      <c r="R25" s="195"/>
+      <c r="S25" s="195"/>
+      <c r="T25" s="195"/>
+      <c r="U25" s="195"/>
+      <c r="V25" s="195"/>
+      <c r="W25" s="195"/>
+      <c r="X25" s="195"/>
+      <c r="Y25" s="195"/>
     </row>
     <row r="221" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B221" s="148"/>
@@ -4987,23 +4987,18 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="26" fitToHeight="4" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" hiddenColumns="1" showRuler="0">
-      <pane xSplit="35.840909090909093" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G529" sqref="G529"/>
-      <colBreaks count="1" manualBreakCount="1">
-        <brk id="17" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.3" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
-      <printOptions horizontalCentered="1"/>
-      <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId2"/>
+    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" scale="85" showAutoFilter="1" hiddenColumns="1" showRuler="0" topLeftCell="A1417">
+      <selection activeCell="M1442" sqref="M1442"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="landscape" horizontalDpi="120" verticalDpi="144" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
@@ -5014,16 +5009,21 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
-    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" scale="85" showAutoFilter="1" hiddenColumns="1" showRuler="0" topLeftCell="A1417">
-      <selection activeCell="M1442" sqref="M1442"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="landscape" horizontalDpi="120" verticalDpi="144" r:id="rId4"/>
+    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" hiddenColumns="1" showRuler="0">
+      <pane xSplit="35.840909090909093" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G529" sqref="G529"/>
+      <colBreaks count="1" manualBreakCount="1">
+        <brk id="17" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.3" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
+      <printOptions horizontalCentered="1"/>
+      <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="26" fitToHeight="4" orientation="portrait" r:id="rId5"/>
@@ -5061,7 +5061,7 @@
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:Y20"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5151,89 +5151,89 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="196"/>
-      <c r="S3" s="196"/>
-      <c r="T3" s="196"/>
-      <c r="U3" s="196"/>
-      <c r="V3" s="196"/>
-      <c r="W3" s="196"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="197"/>
+      <c r="Q3" s="197"/>
+      <c r="R3" s="197"/>
+      <c r="S3" s="197"/>
+      <c r="T3" s="197"/>
+      <c r="U3" s="197"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="197"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="201" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
-      <c r="L4" s="204"/>
-      <c r="M4" s="204"/>
-      <c r="N4" s="204"/>
-      <c r="O4" s="204"/>
-      <c r="P4" s="204"/>
-      <c r="Q4" s="204"/>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="204"/>
-      <c r="X4" s="204"/>
-      <c r="Y4" s="205"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="202"/>
+      <c r="S4" s="202"/>
+      <c r="T4" s="202"/>
+      <c r="U4" s="202"/>
+      <c r="V4" s="202"/>
+      <c r="W4" s="202"/>
+      <c r="X4" s="202"/>
+      <c r="Y4" s="203"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -5388,32 +5388,32 @@
       <c r="Y8" s="135"/>
     </row>
     <row r="9" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="201" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="204"/>
-      <c r="D9" s="204"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="204"/>
-      <c r="H9" s="204"/>
-      <c r="I9" s="204"/>
-      <c r="J9" s="204"/>
-      <c r="K9" s="204"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="204"/>
-      <c r="N9" s="204"/>
-      <c r="O9" s="204"/>
-      <c r="P9" s="204"/>
-      <c r="Q9" s="204"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="204"/>
-      <c r="U9" s="204"/>
-      <c r="V9" s="204"/>
-      <c r="W9" s="204"/>
-      <c r="X9" s="204"/>
-      <c r="Y9" s="205"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="202"/>
+      <c r="J9" s="202"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="202"/>
+      <c r="S9" s="202"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="202"/>
+      <c r="X9" s="202"/>
+      <c r="Y9" s="203"/>
     </row>
     <row r="10" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="141" t="s">
@@ -5568,32 +5568,32 @@
       <c r="Y13" s="135"/>
     </row>
     <row r="14" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="203" t="s">
+      <c r="B14" s="201" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="204"/>
-      <c r="D14" s="204"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="204"/>
-      <c r="G14" s="204"/>
-      <c r="H14" s="204"/>
-      <c r="I14" s="204"/>
-      <c r="J14" s="204"/>
-      <c r="K14" s="204"/>
-      <c r="L14" s="204"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="204"/>
-      <c r="O14" s="204"/>
-      <c r="P14" s="204"/>
-      <c r="Q14" s="204"/>
-      <c r="R14" s="204"/>
-      <c r="S14" s="204"/>
-      <c r="T14" s="204"/>
-      <c r="U14" s="204"/>
-      <c r="V14" s="204"/>
-      <c r="W14" s="204"/>
-      <c r="X14" s="204"/>
-      <c r="Y14" s="205"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="202"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+      <c r="Q14" s="202"/>
+      <c r="R14" s="202"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
+      <c r="U14" s="202"/>
+      <c r="V14" s="202"/>
+      <c r="W14" s="202"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="203"/>
     </row>
     <row r="15" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
@@ -5748,32 +5748,32 @@
       <c r="Y18" s="173"/>
     </row>
     <row r="19" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="203" t="s">
+      <c r="B19" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="204"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="204"/>
-      <c r="F19" s="204"/>
-      <c r="G19" s="204"/>
-      <c r="H19" s="204"/>
-      <c r="I19" s="204"/>
-      <c r="J19" s="204"/>
-      <c r="K19" s="204"/>
-      <c r="L19" s="204"/>
-      <c r="M19" s="204"/>
-      <c r="N19" s="204"/>
-      <c r="O19" s="204"/>
-      <c r="P19" s="204"/>
-      <c r="Q19" s="204"/>
-      <c r="R19" s="204"/>
-      <c r="S19" s="204"/>
-      <c r="T19" s="204"/>
-      <c r="U19" s="204"/>
-      <c r="V19" s="204"/>
-      <c r="W19" s="204"/>
-      <c r="X19" s="204"/>
-      <c r="Y19" s="205"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="202"/>
+      <c r="M19" s="202"/>
+      <c r="N19" s="202"/>
+      <c r="O19" s="202"/>
+      <c r="P19" s="202"/>
+      <c r="Q19" s="202"/>
+      <c r="R19" s="202"/>
+      <c r="S19" s="202"/>
+      <c r="T19" s="202"/>
+      <c r="U19" s="202"/>
+      <c r="V19" s="202"/>
+      <c r="W19" s="202"/>
+      <c r="X19" s="202"/>
+      <c r="Y19" s="203"/>
     </row>
     <row r="20" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="141" t="s">
@@ -5876,117 +5876,114 @@
       <c r="Y21" s="180"/>
     </row>
     <row r="22" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="195"/>
-      <c r="C22" s="195"/>
-      <c r="D22" s="195"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="195"/>
-      <c r="L22" s="195"/>
-      <c r="M22" s="195"/>
-      <c r="N22" s="195"/>
-      <c r="O22" s="195"/>
-      <c r="P22" s="195"/>
-      <c r="Q22" s="195"/>
-      <c r="R22" s="195"/>
-      <c r="S22" s="195"/>
-      <c r="T22" s="195"/>
-      <c r="U22" s="195"/>
-      <c r="V22" s="195"/>
-      <c r="W22" s="195"/>
-      <c r="X22" s="195"/>
-      <c r="Y22" s="195"/>
+      <c r="B22" s="196"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="196"/>
+      <c r="E22" s="196"/>
+      <c r="F22" s="196"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+      <c r="K22" s="196"/>
+      <c r="L22" s="196"/>
+      <c r="M22" s="196"/>
+      <c r="N22" s="196"/>
+      <c r="O22" s="196"/>
+      <c r="P22" s="196"/>
+      <c r="Q22" s="196"/>
+      <c r="R22" s="196"/>
+      <c r="S22" s="196"/>
+      <c r="T22" s="196"/>
+      <c r="U22" s="196"/>
+      <c r="V22" s="196"/>
+      <c r="W22" s="196"/>
+      <c r="X22" s="196"/>
+      <c r="Y22" s="196"/>
     </row>
     <row r="23" spans="2:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="198"/>
-      <c r="D23" s="198"/>
-      <c r="E23" s="198"/>
-      <c r="F23" s="198"/>
-      <c r="G23" s="198"/>
-      <c r="H23" s="198"/>
-      <c r="I23" s="198"/>
-      <c r="J23" s="198"/>
-      <c r="K23" s="198"/>
-      <c r="L23" s="198"/>
-      <c r="M23" s="198"/>
-      <c r="N23" s="198"/>
-      <c r="O23" s="198"/>
-      <c r="P23" s="198"/>
-      <c r="Q23" s="198"/>
-      <c r="R23" s="198"/>
-      <c r="S23" s="198"/>
-      <c r="T23" s="198"/>
-      <c r="U23" s="198"/>
-      <c r="V23" s="198"/>
-      <c r="W23" s="198"/>
-      <c r="X23" s="198"/>
-      <c r="Y23" s="198"/>
+      <c r="B23" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="199"/>
+      <c r="D23" s="199"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
+      <c r="G23" s="199"/>
+      <c r="H23" s="199"/>
+      <c r="I23" s="199"/>
+      <c r="J23" s="199"/>
+      <c r="K23" s="199"/>
+      <c r="L23" s="199"/>
+      <c r="M23" s="199"/>
+      <c r="N23" s="199"/>
+      <c r="O23" s="199"/>
+      <c r="P23" s="199"/>
+      <c r="Q23" s="199"/>
+      <c r="R23" s="199"/>
+      <c r="S23" s="199"/>
+      <c r="T23" s="199"/>
+      <c r="U23" s="199"/>
+      <c r="V23" s="199"/>
+      <c r="W23" s="199"/>
+      <c r="X23" s="199"/>
+      <c r="Y23" s="199"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C24" s="199"/>
-      <c r="D24" s="199"/>
-      <c r="E24" s="199"/>
-      <c r="F24" s="199"/>
-      <c r="G24" s="199"/>
-      <c r="H24" s="199"/>
-      <c r="I24" s="199"/>
-      <c r="J24" s="199"/>
-      <c r="K24" s="199"/>
-      <c r="L24" s="199"/>
-      <c r="M24" s="199"/>
-      <c r="N24" s="199"/>
-      <c r="O24" s="199"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="199"/>
-      <c r="R24" s="199"/>
-      <c r="S24" s="199"/>
-      <c r="T24" s="199"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="199"/>
-      <c r="W24" s="199"/>
-      <c r="X24" s="199"/>
-      <c r="Y24" s="199"/>
+      <c r="B24" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="200"/>
+      <c r="I24" s="200"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="200"/>
+      <c r="L24" s="200"/>
+      <c r="M24" s="200"/>
+      <c r="N24" s="200"/>
+      <c r="O24" s="200"/>
+      <c r="P24" s="200"/>
+      <c r="Q24" s="200"/>
+      <c r="R24" s="200"/>
+      <c r="S24" s="200"/>
+      <c r="T24" s="200"/>
+      <c r="U24" s="200"/>
+      <c r="V24" s="200"/>
+      <c r="W24" s="200"/>
+      <c r="X24" s="200"/>
+      <c r="Y24" s="200"/>
     </row>
     <row r="25" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="194"/>
-      <c r="K25" s="194"/>
-      <c r="L25" s="194"/>
-      <c r="M25" s="194"/>
-      <c r="N25" s="194"/>
-      <c r="O25" s="194"/>
-      <c r="P25" s="194"/>
-      <c r="Q25" s="194"/>
-      <c r="R25" s="194"/>
-      <c r="S25" s="194"/>
-      <c r="T25" s="194"/>
-      <c r="U25" s="194"/>
-      <c r="V25" s="194"/>
-      <c r="W25" s="194"/>
-      <c r="X25" s="194"/>
-      <c r="Y25" s="194"/>
+      <c r="B25" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="195"/>
+      <c r="D25" s="195"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="195"/>
+      <c r="H25" s="195"/>
+      <c r="I25" s="195"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="N25" s="195"/>
+      <c r="O25" s="195"/>
+      <c r="P25" s="195"/>
+      <c r="Q25" s="195"/>
+      <c r="R25" s="195"/>
+      <c r="S25" s="195"/>
+      <c r="T25" s="195"/>
+      <c r="U25" s="195"/>
+      <c r="V25" s="195"/>
+      <c r="W25" s="195"/>
+      <c r="X25" s="195"/>
+      <c r="Y25" s="195"/>
     </row>
     <row r="26" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="138"/>
@@ -6015,82 +6012,82 @@
       <c r="Y26" s="138"/>
     </row>
     <row r="27" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="198"/>
-      <c r="C27" s="199"/>
-      <c r="D27" s="199"/>
-      <c r="E27" s="210"/>
-      <c r="F27" s="199"/>
-      <c r="G27" s="199"/>
-      <c r="H27" s="199"/>
-      <c r="I27" s="199"/>
-      <c r="J27" s="199"/>
-      <c r="K27" s="199"/>
-      <c r="L27" s="199"/>
-      <c r="M27" s="199"/>
-      <c r="N27" s="210"/>
-      <c r="O27" s="210"/>
-      <c r="P27" s="210"/>
-      <c r="Q27" s="210"/>
-      <c r="R27" s="210"/>
-      <c r="S27" s="210"/>
-      <c r="T27" s="210"/>
-      <c r="U27" s="210"/>
-      <c r="V27" s="210"/>
-      <c r="W27" s="210"/>
-      <c r="X27" s="199"/>
-      <c r="Y27" s="199"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="200"/>
+      <c r="D27" s="200"/>
+      <c r="E27" s="208"/>
+      <c r="F27" s="200"/>
+      <c r="G27" s="200"/>
+      <c r="H27" s="200"/>
+      <c r="I27" s="200"/>
+      <c r="J27" s="200"/>
+      <c r="K27" s="200"/>
+      <c r="L27" s="200"/>
+      <c r="M27" s="200"/>
+      <c r="N27" s="208"/>
+      <c r="O27" s="208"/>
+      <c r="P27" s="208"/>
+      <c r="Q27" s="208"/>
+      <c r="R27" s="208"/>
+      <c r="S27" s="208"/>
+      <c r="T27" s="208"/>
+      <c r="U27" s="208"/>
+      <c r="V27" s="208"/>
+      <c r="W27" s="208"/>
+      <c r="X27" s="200"/>
+      <c r="Y27" s="200"/>
     </row>
     <row r="28" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="199"/>
-      <c r="C28" s="199"/>
-      <c r="D28" s="199"/>
-      <c r="E28" s="210"/>
-      <c r="F28" s="199"/>
-      <c r="G28" s="199"/>
-      <c r="H28" s="199"/>
-      <c r="I28" s="199"/>
-      <c r="J28" s="199"/>
-      <c r="K28" s="199"/>
-      <c r="L28" s="199"/>
-      <c r="M28" s="199"/>
-      <c r="N28" s="210"/>
-      <c r="O28" s="210"/>
-      <c r="P28" s="210"/>
-      <c r="Q28" s="210"/>
-      <c r="R28" s="210"/>
-      <c r="S28" s="210"/>
-      <c r="T28" s="210"/>
-      <c r="U28" s="210"/>
-      <c r="V28" s="210"/>
-      <c r="W28" s="210"/>
-      <c r="X28" s="199"/>
-      <c r="Y28" s="199"/>
+      <c r="B28" s="200"/>
+      <c r="C28" s="200"/>
+      <c r="D28" s="200"/>
+      <c r="E28" s="208"/>
+      <c r="F28" s="200"/>
+      <c r="G28" s="200"/>
+      <c r="H28" s="200"/>
+      <c r="I28" s="200"/>
+      <c r="J28" s="200"/>
+      <c r="K28" s="200"/>
+      <c r="L28" s="200"/>
+      <c r="M28" s="200"/>
+      <c r="N28" s="208"/>
+      <c r="O28" s="208"/>
+      <c r="P28" s="208"/>
+      <c r="Q28" s="208"/>
+      <c r="R28" s="208"/>
+      <c r="S28" s="208"/>
+      <c r="T28" s="208"/>
+      <c r="U28" s="208"/>
+      <c r="V28" s="208"/>
+      <c r="W28" s="208"/>
+      <c r="X28" s="200"/>
+      <c r="Y28" s="200"/>
     </row>
     <row r="29" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="194"/>
-      <c r="C29" s="194"/>
-      <c r="D29" s="194"/>
-      <c r="E29" s="210"/>
-      <c r="F29" s="194"/>
-      <c r="G29" s="194"/>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="194"/>
-      <c r="K29" s="194"/>
-      <c r="L29" s="194"/>
-      <c r="M29" s="194"/>
-      <c r="N29" s="210"/>
-      <c r="O29" s="210"/>
-      <c r="P29" s="210"/>
-      <c r="Q29" s="210"/>
-      <c r="R29" s="210"/>
-      <c r="S29" s="210"/>
-      <c r="T29" s="210"/>
-      <c r="U29" s="210"/>
-      <c r="V29" s="210"/>
-      <c r="W29" s="210"/>
-      <c r="X29" s="194"/>
-      <c r="Y29" s="194"/>
+      <c r="B29" s="195"/>
+      <c r="C29" s="195"/>
+      <c r="D29" s="195"/>
+      <c r="E29" s="208"/>
+      <c r="F29" s="195"/>
+      <c r="G29" s="195"/>
+      <c r="H29" s="195"/>
+      <c r="I29" s="195"/>
+      <c r="J29" s="195"/>
+      <c r="K29" s="195"/>
+      <c r="L29" s="195"/>
+      <c r="M29" s="195"/>
+      <c r="N29" s="208"/>
+      <c r="O29" s="208"/>
+      <c r="P29" s="208"/>
+      <c r="Q29" s="208"/>
+      <c r="R29" s="208"/>
+      <c r="S29" s="208"/>
+      <c r="T29" s="208"/>
+      <c r="U29" s="208"/>
+      <c r="V29" s="208"/>
+      <c r="W29" s="208"/>
+      <c r="X29" s="195"/>
+      <c r="Y29" s="195"/>
     </row>
     <row r="222" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B222" s="148"/>
@@ -6121,11 +6118,6 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="13">
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="B9:Y9"/>
-    <mergeCell ref="B14:Y14"/>
     <mergeCell ref="B19:Y19"/>
     <mergeCell ref="B27:Y27"/>
     <mergeCell ref="B28:Y28"/>
@@ -6134,6 +6126,11 @@
     <mergeCell ref="B25:Y25"/>
     <mergeCell ref="B23:Y23"/>
     <mergeCell ref="B22:Y22"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B9:Y9"/>
+    <mergeCell ref="B14:Y14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6153,7 +6150,7 @@
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:Y20"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6243,89 +6240,89 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="196"/>
-      <c r="S3" s="196"/>
-      <c r="T3" s="196"/>
-      <c r="U3" s="196"/>
-      <c r="V3" s="196"/>
-      <c r="W3" s="196"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="197"/>
+      <c r="Q3" s="197"/>
+      <c r="R3" s="197"/>
+      <c r="S3" s="197"/>
+      <c r="T3" s="197"/>
+      <c r="U3" s="197"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="197"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
-      <c r="L4" s="204"/>
-      <c r="M4" s="204"/>
-      <c r="N4" s="204"/>
-      <c r="O4" s="204"/>
-      <c r="P4" s="204"/>
-      <c r="Q4" s="204"/>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="204"/>
-      <c r="X4" s="204"/>
-      <c r="Y4" s="205"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="202"/>
+      <c r="S4" s="202"/>
+      <c r="T4" s="202"/>
+      <c r="U4" s="202"/>
+      <c r="V4" s="202"/>
+      <c r="W4" s="202"/>
+      <c r="X4" s="202"/>
+      <c r="Y4" s="203"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -6480,32 +6477,32 @@
       <c r="Y8" s="135"/>
     </row>
     <row r="9" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="201" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="204"/>
-      <c r="D9" s="204"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="204"/>
-      <c r="H9" s="204"/>
-      <c r="I9" s="204"/>
-      <c r="J9" s="204"/>
-      <c r="K9" s="204"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="204"/>
-      <c r="N9" s="204"/>
-      <c r="O9" s="204"/>
-      <c r="P9" s="204"/>
-      <c r="Q9" s="204"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="204"/>
-      <c r="U9" s="204"/>
-      <c r="V9" s="204"/>
-      <c r="W9" s="204"/>
-      <c r="X9" s="204"/>
-      <c r="Y9" s="205"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="202"/>
+      <c r="J9" s="202"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="202"/>
+      <c r="S9" s="202"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="202"/>
+      <c r="X9" s="202"/>
+      <c r="Y9" s="203"/>
     </row>
     <row r="10" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="141" t="s">
@@ -6660,32 +6657,32 @@
       <c r="Y13" s="135"/>
     </row>
     <row r="14" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="203" t="s">
+      <c r="B14" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="204"/>
-      <c r="D14" s="204"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="204"/>
-      <c r="G14" s="204"/>
-      <c r="H14" s="204"/>
-      <c r="I14" s="204"/>
-      <c r="J14" s="204"/>
-      <c r="K14" s="204"/>
-      <c r="L14" s="204"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="204"/>
-      <c r="O14" s="204"/>
-      <c r="P14" s="204"/>
-      <c r="Q14" s="204"/>
-      <c r="R14" s="204"/>
-      <c r="S14" s="204"/>
-      <c r="T14" s="204"/>
-      <c r="U14" s="204"/>
-      <c r="V14" s="204"/>
-      <c r="W14" s="204"/>
-      <c r="X14" s="204"/>
-      <c r="Y14" s="205"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="202"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+      <c r="Q14" s="202"/>
+      <c r="R14" s="202"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
+      <c r="U14" s="202"/>
+      <c r="V14" s="202"/>
+      <c r="W14" s="202"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="203"/>
     </row>
     <row r="15" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
@@ -6840,32 +6837,32 @@
       <c r="Y18" s="137"/>
     </row>
     <row r="19" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="203" t="s">
+      <c r="B19" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="204"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="204"/>
-      <c r="F19" s="204"/>
-      <c r="G19" s="204"/>
-      <c r="H19" s="204"/>
-      <c r="I19" s="204"/>
-      <c r="J19" s="204"/>
-      <c r="K19" s="204"/>
-      <c r="L19" s="204"/>
-      <c r="M19" s="204"/>
-      <c r="N19" s="204"/>
-      <c r="O19" s="204"/>
-      <c r="P19" s="204"/>
-      <c r="Q19" s="204"/>
-      <c r="R19" s="204"/>
-      <c r="S19" s="204"/>
-      <c r="T19" s="204"/>
-      <c r="U19" s="204"/>
-      <c r="V19" s="204"/>
-      <c r="W19" s="204"/>
-      <c r="X19" s="204"/>
-      <c r="Y19" s="205"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="202"/>
+      <c r="M19" s="202"/>
+      <c r="N19" s="202"/>
+      <c r="O19" s="202"/>
+      <c r="P19" s="202"/>
+      <c r="Q19" s="202"/>
+      <c r="R19" s="202"/>
+      <c r="S19" s="202"/>
+      <c r="T19" s="202"/>
+      <c r="U19" s="202"/>
+      <c r="V19" s="202"/>
+      <c r="W19" s="202"/>
+      <c r="X19" s="202"/>
+      <c r="Y19" s="203"/>
     </row>
     <row r="20" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="141" t="s">
@@ -6968,117 +6965,114 @@
       <c r="Y21" s="180"/>
     </row>
     <row r="22" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="195"/>
-      <c r="C22" s="195"/>
-      <c r="D22" s="195"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="195"/>
-      <c r="L22" s="195"/>
-      <c r="M22" s="195"/>
-      <c r="N22" s="195"/>
-      <c r="O22" s="195"/>
-      <c r="P22" s="195"/>
-      <c r="Q22" s="195"/>
-      <c r="R22" s="195"/>
-      <c r="S22" s="195"/>
-      <c r="T22" s="195"/>
-      <c r="U22" s="195"/>
-      <c r="V22" s="195"/>
-      <c r="W22" s="195"/>
-      <c r="X22" s="195"/>
-      <c r="Y22" s="195"/>
+      <c r="B22" s="196"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="196"/>
+      <c r="E22" s="196"/>
+      <c r="F22" s="196"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+      <c r="K22" s="196"/>
+      <c r="L22" s="196"/>
+      <c r="M22" s="196"/>
+      <c r="N22" s="196"/>
+      <c r="O22" s="196"/>
+      <c r="P22" s="196"/>
+      <c r="Q22" s="196"/>
+      <c r="R22" s="196"/>
+      <c r="S22" s="196"/>
+      <c r="T22" s="196"/>
+      <c r="U22" s="196"/>
+      <c r="V22" s="196"/>
+      <c r="W22" s="196"/>
+      <c r="X22" s="196"/>
+      <c r="Y22" s="196"/>
     </row>
     <row r="23" spans="2:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="198"/>
-      <c r="D23" s="198"/>
-      <c r="E23" s="198"/>
-      <c r="F23" s="198"/>
-      <c r="G23" s="198"/>
-      <c r="H23" s="198"/>
-      <c r="I23" s="198"/>
-      <c r="J23" s="198"/>
-      <c r="K23" s="198"/>
-      <c r="L23" s="198"/>
-      <c r="M23" s="198"/>
-      <c r="N23" s="198"/>
-      <c r="O23" s="198"/>
-      <c r="P23" s="198"/>
-      <c r="Q23" s="198"/>
-      <c r="R23" s="198"/>
-      <c r="S23" s="198"/>
-      <c r="T23" s="198"/>
-      <c r="U23" s="198"/>
-      <c r="V23" s="198"/>
-      <c r="W23" s="198"/>
-      <c r="X23" s="198"/>
-      <c r="Y23" s="198"/>
+      <c r="B23" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="199"/>
+      <c r="D23" s="199"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
+      <c r="G23" s="199"/>
+      <c r="H23" s="199"/>
+      <c r="I23" s="199"/>
+      <c r="J23" s="199"/>
+      <c r="K23" s="199"/>
+      <c r="L23" s="199"/>
+      <c r="M23" s="199"/>
+      <c r="N23" s="199"/>
+      <c r="O23" s="199"/>
+      <c r="P23" s="199"/>
+      <c r="Q23" s="199"/>
+      <c r="R23" s="199"/>
+      <c r="S23" s="199"/>
+      <c r="T23" s="199"/>
+      <c r="U23" s="199"/>
+      <c r="V23" s="199"/>
+      <c r="W23" s="199"/>
+      <c r="X23" s="199"/>
+      <c r="Y23" s="199"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C24" s="199"/>
-      <c r="D24" s="199"/>
-      <c r="E24" s="199"/>
-      <c r="F24" s="199"/>
-      <c r="G24" s="199"/>
-      <c r="H24" s="199"/>
-      <c r="I24" s="199"/>
-      <c r="J24" s="199"/>
-      <c r="K24" s="199"/>
-      <c r="L24" s="199"/>
-      <c r="M24" s="199"/>
-      <c r="N24" s="199"/>
-      <c r="O24" s="199"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="199"/>
-      <c r="R24" s="199"/>
-      <c r="S24" s="199"/>
-      <c r="T24" s="199"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="199"/>
-      <c r="W24" s="199"/>
-      <c r="X24" s="199"/>
-      <c r="Y24" s="199"/>
+      <c r="B24" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="200"/>
+      <c r="I24" s="200"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="200"/>
+      <c r="L24" s="200"/>
+      <c r="M24" s="200"/>
+      <c r="N24" s="200"/>
+      <c r="O24" s="200"/>
+      <c r="P24" s="200"/>
+      <c r="Q24" s="200"/>
+      <c r="R24" s="200"/>
+      <c r="S24" s="200"/>
+      <c r="T24" s="200"/>
+      <c r="U24" s="200"/>
+      <c r="V24" s="200"/>
+      <c r="W24" s="200"/>
+      <c r="X24" s="200"/>
+      <c r="Y24" s="200"/>
     </row>
     <row r="25" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="194"/>
-      <c r="K25" s="194"/>
-      <c r="L25" s="194"/>
-      <c r="M25" s="194"/>
-      <c r="N25" s="194"/>
-      <c r="O25" s="194"/>
-      <c r="P25" s="194"/>
-      <c r="Q25" s="194"/>
-      <c r="R25" s="194"/>
-      <c r="S25" s="194"/>
-      <c r="T25" s="194"/>
-      <c r="U25" s="194"/>
-      <c r="V25" s="194"/>
-      <c r="W25" s="194"/>
-      <c r="X25" s="194"/>
-      <c r="Y25" s="194"/>
+      <c r="B25" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="195"/>
+      <c r="D25" s="195"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="195"/>
+      <c r="H25" s="195"/>
+      <c r="I25" s="195"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="N25" s="195"/>
+      <c r="O25" s="195"/>
+      <c r="P25" s="195"/>
+      <c r="Q25" s="195"/>
+      <c r="R25" s="195"/>
+      <c r="S25" s="195"/>
+      <c r="T25" s="195"/>
+      <c r="U25" s="195"/>
+      <c r="V25" s="195"/>
+      <c r="W25" s="195"/>
+      <c r="X25" s="195"/>
+      <c r="Y25" s="195"/>
     </row>
     <row r="26" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X26" s="108"/>
@@ -10143,16 +10137,16 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="10">
+    <mergeCell ref="B25:Y25"/>
+    <mergeCell ref="B24:Y24"/>
+    <mergeCell ref="B23:Y23"/>
+    <mergeCell ref="B22:Y22"/>
+    <mergeCell ref="B19:Y19"/>
     <mergeCell ref="B3:Y3"/>
     <mergeCell ref="B2:Y2"/>
     <mergeCell ref="B4:Y4"/>
     <mergeCell ref="B9:Y9"/>
     <mergeCell ref="B14:Y14"/>
-    <mergeCell ref="B25:Y25"/>
-    <mergeCell ref="B24:Y24"/>
-    <mergeCell ref="B23:Y23"/>
-    <mergeCell ref="B22:Y22"/>
-    <mergeCell ref="B19:Y19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10175,7 +10169,7 @@
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:Y5"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10265,61 +10259,61 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1 &amp; " за " &amp; Главная!A2 &amp; " " &amp; Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="211"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="197"/>
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="212"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="196"/>
-      <c r="R3" s="196"/>
-      <c r="S3" s="196"/>
-      <c r="T3" s="196"/>
-      <c r="U3" s="196"/>
-      <c r="V3" s="196"/>
-      <c r="W3" s="196"/>
-      <c r="X3" s="211"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="197"/>
+      <c r="Q3" s="197"/>
+      <c r="R3" s="197"/>
+      <c r="S3" s="197"/>
+      <c r="T3" s="197"/>
+      <c r="U3" s="197"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="197"/>
+      <c r="X3" s="212"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="2:25" s="110" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="150"/>
@@ -10448,117 +10442,114 @@
       <c r="Y6" s="180"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="195"/>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195"/>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="195"/>
-      <c r="I7" s="195"/>
-      <c r="J7" s="195"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="195"/>
-      <c r="M7" s="195"/>
-      <c r="N7" s="195"/>
-      <c r="O7" s="195"/>
-      <c r="P7" s="195"/>
-      <c r="Q7" s="195"/>
-      <c r="R7" s="195"/>
-      <c r="S7" s="195"/>
-      <c r="T7" s="195"/>
-      <c r="U7" s="195"/>
-      <c r="V7" s="195"/>
-      <c r="W7" s="195"/>
-      <c r="X7" s="195"/>
-      <c r="Y7" s="195"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="196"/>
+      <c r="E7" s="196"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="196"/>
+      <c r="H7" s="196"/>
+      <c r="I7" s="196"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="196"/>
+      <c r="N7" s="196"/>
+      <c r="O7" s="196"/>
+      <c r="P7" s="196"/>
+      <c r="Q7" s="196"/>
+      <c r="R7" s="196"/>
+      <c r="S7" s="196"/>
+      <c r="T7" s="196"/>
+      <c r="U7" s="196"/>
+      <c r="V7" s="196"/>
+      <c r="W7" s="196"/>
+      <c r="X7" s="196"/>
+      <c r="Y7" s="196"/>
     </row>
     <row r="8" spans="2:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C8" s="198"/>
-      <c r="D8" s="198"/>
-      <c r="E8" s="198"/>
-      <c r="F8" s="198"/>
-      <c r="G8" s="198"/>
-      <c r="H8" s="198"/>
-      <c r="I8" s="198"/>
-      <c r="J8" s="198"/>
-      <c r="K8" s="198"/>
-      <c r="L8" s="198"/>
-      <c r="M8" s="198"/>
-      <c r="N8" s="198"/>
-      <c r="O8" s="198"/>
-      <c r="P8" s="198"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="198"/>
-      <c r="S8" s="198"/>
-      <c r="T8" s="198"/>
-      <c r="U8" s="198"/>
-      <c r="V8" s="198"/>
-      <c r="W8" s="198"/>
-      <c r="X8" s="198"/>
-      <c r="Y8" s="198"/>
+      <c r="B8" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="199"/>
+      <c r="D8" s="199"/>
+      <c r="E8" s="199"/>
+      <c r="F8" s="199"/>
+      <c r="G8" s="199"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="199"/>
+      <c r="L8" s="199"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="199"/>
+      <c r="R8" s="199"/>
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="199"/>
+      <c r="W8" s="199"/>
+      <c r="X8" s="199"/>
+      <c r="Y8" s="199"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="199"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="199"/>
-      <c r="H9" s="199"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="199"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="199"/>
-      <c r="M9" s="199"/>
-      <c r="N9" s="199"/>
-      <c r="O9" s="199"/>
-      <c r="P9" s="199"/>
-      <c r="Q9" s="199"/>
-      <c r="R9" s="199"/>
-      <c r="S9" s="199"/>
-      <c r="T9" s="199"/>
-      <c r="U9" s="199"/>
-      <c r="V9" s="199"/>
-      <c r="W9" s="199"/>
-      <c r="X9" s="199"/>
-      <c r="Y9" s="199"/>
+      <c r="B9" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="200"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
+      <c r="L9" s="200"/>
+      <c r="M9" s="200"/>
+      <c r="N9" s="200"/>
+      <c r="O9" s="200"/>
+      <c r="P9" s="200"/>
+      <c r="Q9" s="200"/>
+      <c r="R9" s="200"/>
+      <c r="S9" s="200"/>
+      <c r="T9" s="200"/>
+      <c r="U9" s="200"/>
+      <c r="V9" s="200"/>
+      <c r="W9" s="200"/>
+      <c r="X9" s="200"/>
+      <c r="Y9" s="200"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C10" s="194"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="194"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="194"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="194"/>
-      <c r="M10" s="194"/>
-      <c r="N10" s="194"/>
-      <c r="O10" s="194"/>
-      <c r="P10" s="194"/>
-      <c r="Q10" s="194"/>
-      <c r="R10" s="194"/>
-      <c r="S10" s="194"/>
-      <c r="T10" s="194"/>
-      <c r="U10" s="194"/>
-      <c r="V10" s="194"/>
-      <c r="W10" s="194"/>
-      <c r="X10" s="194"/>
-      <c r="Y10" s="194"/>
+      <c r="B10" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="195"/>
+      <c r="I10" s="195"/>
+      <c r="J10" s="195"/>
+      <c r="K10" s="195"/>
+      <c r="L10" s="195"/>
+      <c r="M10" s="195"/>
+      <c r="N10" s="195"/>
+      <c r="O10" s="195"/>
+      <c r="P10" s="195"/>
+      <c r="Q10" s="195"/>
+      <c r="R10" s="195"/>
+      <c r="S10" s="195"/>
+      <c r="T10" s="195"/>
+      <c r="U10" s="195"/>
+      <c r="V10" s="195"/>
+      <c r="W10" s="195"/>
+      <c r="X10" s="195"/>
+      <c r="Y10" s="195"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="138"/>
@@ -10587,82 +10578,82 @@
       <c r="Y11" s="138"/>
     </row>
     <row r="12" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="198"/>
-      <c r="C12" s="199"/>
-      <c r="D12" s="199"/>
-      <c r="E12" s="199"/>
-      <c r="F12" s="199"/>
-      <c r="G12" s="199"/>
-      <c r="H12" s="199"/>
-      <c r="I12" s="199"/>
-      <c r="J12" s="199"/>
-      <c r="K12" s="199"/>
-      <c r="L12" s="199"/>
-      <c r="M12" s="199"/>
-      <c r="N12" s="210"/>
-      <c r="O12" s="210"/>
-      <c r="P12" s="210"/>
-      <c r="Q12" s="210"/>
-      <c r="R12" s="210"/>
-      <c r="S12" s="210"/>
-      <c r="T12" s="210"/>
-      <c r="U12" s="210"/>
-      <c r="V12" s="210"/>
-      <c r="W12" s="210"/>
-      <c r="X12" s="199"/>
-      <c r="Y12" s="199"/>
+      <c r="B12" s="199"/>
+      <c r="C12" s="200"/>
+      <c r="D12" s="200"/>
+      <c r="E12" s="200"/>
+      <c r="F12" s="200"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="200"/>
+      <c r="I12" s="200"/>
+      <c r="J12" s="200"/>
+      <c r="K12" s="200"/>
+      <c r="L12" s="200"/>
+      <c r="M12" s="200"/>
+      <c r="N12" s="208"/>
+      <c r="O12" s="208"/>
+      <c r="P12" s="208"/>
+      <c r="Q12" s="208"/>
+      <c r="R12" s="208"/>
+      <c r="S12" s="208"/>
+      <c r="T12" s="208"/>
+      <c r="U12" s="208"/>
+      <c r="V12" s="208"/>
+      <c r="W12" s="208"/>
+      <c r="X12" s="200"/>
+      <c r="Y12" s="200"/>
     </row>
     <row r="13" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="199"/>
-      <c r="C13" s="199"/>
-      <c r="D13" s="199"/>
-      <c r="E13" s="199"/>
-      <c r="F13" s="199"/>
-      <c r="G13" s="199"/>
-      <c r="H13" s="199"/>
-      <c r="I13" s="199"/>
-      <c r="J13" s="199"/>
-      <c r="K13" s="199"/>
-      <c r="L13" s="199"/>
-      <c r="M13" s="199"/>
-      <c r="N13" s="210"/>
-      <c r="O13" s="210"/>
-      <c r="P13" s="210"/>
-      <c r="Q13" s="210"/>
-      <c r="R13" s="210"/>
-      <c r="S13" s="210"/>
-      <c r="T13" s="210"/>
-      <c r="U13" s="210"/>
-      <c r="V13" s="210"/>
-      <c r="W13" s="210"/>
-      <c r="X13" s="199"/>
-      <c r="Y13" s="199"/>
+      <c r="B13" s="200"/>
+      <c r="C13" s="200"/>
+      <c r="D13" s="200"/>
+      <c r="E13" s="200"/>
+      <c r="F13" s="200"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="200"/>
+      <c r="I13" s="200"/>
+      <c r="J13" s="200"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="200"/>
+      <c r="M13" s="200"/>
+      <c r="N13" s="208"/>
+      <c r="O13" s="208"/>
+      <c r="P13" s="208"/>
+      <c r="Q13" s="208"/>
+      <c r="R13" s="208"/>
+      <c r="S13" s="208"/>
+      <c r="T13" s="208"/>
+      <c r="U13" s="208"/>
+      <c r="V13" s="208"/>
+      <c r="W13" s="208"/>
+      <c r="X13" s="200"/>
+      <c r="Y13" s="200"/>
     </row>
     <row r="14" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="194"/>
-      <c r="M14" s="194"/>
-      <c r="N14" s="210"/>
-      <c r="O14" s="210"/>
-      <c r="P14" s="210"/>
-      <c r="Q14" s="210"/>
-      <c r="R14" s="210"/>
-      <c r="S14" s="210"/>
-      <c r="T14" s="210"/>
-      <c r="U14" s="210"/>
-      <c r="V14" s="210"/>
-      <c r="W14" s="210"/>
-      <c r="X14" s="194"/>
-      <c r="Y14" s="194"/>
+      <c r="B14" s="195"/>
+      <c r="C14" s="195"/>
+      <c r="D14" s="195"/>
+      <c r="E14" s="195"/>
+      <c r="F14" s="195"/>
+      <c r="G14" s="195"/>
+      <c r="H14" s="195"/>
+      <c r="I14" s="195"/>
+      <c r="J14" s="195"/>
+      <c r="K14" s="195"/>
+      <c r="L14" s="195"/>
+      <c r="M14" s="195"/>
+      <c r="N14" s="208"/>
+      <c r="O14" s="208"/>
+      <c r="P14" s="208"/>
+      <c r="Q14" s="208"/>
+      <c r="R14" s="208"/>
+      <c r="S14" s="208"/>
+      <c r="T14" s="208"/>
+      <c r="U14" s="208"/>
+      <c r="V14" s="208"/>
+      <c r="W14" s="208"/>
+      <c r="X14" s="195"/>
+      <c r="Y14" s="195"/>
     </row>
     <row r="15" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X15" s="108"/>
@@ -13495,10 +13486,10 @@
   </sheetPr>
   <dimension ref="B1:Y954"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K110" sqref="K110"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13588,89 +13579,89 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="196" t="str">
+      <c r="B2" s="197" t="str">
         <f>Главная!A1&amp;" за "&amp;Главная!A2&amp;" "&amp;Главная!G2</f>
         <v>Ведомость контрольных занятий за апрель 2014 года</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="197"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="197"/>
-      <c r="W2" s="197"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="198"/>
+      <c r="W2" s="198"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="197"/>
-      <c r="O3" s="197"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="197"/>
-      <c r="R3" s="197"/>
-      <c r="S3" s="197"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="197"/>
-      <c r="V3" s="197"/>
-      <c r="W3" s="197"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="198"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="198"/>
+      <c r="Q3" s="198"/>
+      <c r="R3" s="198"/>
+      <c r="S3" s="198"/>
+      <c r="T3" s="198"/>
+      <c r="U3" s="198"/>
+      <c r="V3" s="198"/>
+      <c r="W3" s="198"/>
+      <c r="X3" s="197"/>
+      <c r="Y3" s="197"/>
     </row>
     <row r="4" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="201" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
-      <c r="L4" s="204"/>
-      <c r="M4" s="204"/>
-      <c r="N4" s="204"/>
-      <c r="O4" s="204"/>
-      <c r="P4" s="204"/>
-      <c r="Q4" s="204"/>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="204"/>
-      <c r="X4" s="204"/>
-      <c r="Y4" s="205"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="202"/>
+      <c r="S4" s="202"/>
+      <c r="T4" s="202"/>
+      <c r="U4" s="202"/>
+      <c r="V4" s="202"/>
+      <c r="W4" s="202"/>
+      <c r="X4" s="202"/>
+      <c r="Y4" s="203"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -13825,32 +13816,32 @@
       <c r="Y8" s="135"/>
     </row>
     <row r="9" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="201" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="204"/>
-      <c r="D9" s="204"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="204"/>
-      <c r="H9" s="204"/>
-      <c r="I9" s="204"/>
-      <c r="J9" s="204"/>
-      <c r="K9" s="204"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="204"/>
-      <c r="N9" s="204"/>
-      <c r="O9" s="204"/>
-      <c r="P9" s="204"/>
-      <c r="Q9" s="204"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="204"/>
-      <c r="U9" s="204"/>
-      <c r="V9" s="204"/>
-      <c r="W9" s="204"/>
-      <c r="X9" s="204"/>
-      <c r="Y9" s="205"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="202"/>
+      <c r="J9" s="202"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="202"/>
+      <c r="S9" s="202"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="202"/>
+      <c r="X9" s="202"/>
+      <c r="Y9" s="203"/>
     </row>
     <row r="10" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="141" t="s">
@@ -14005,32 +13996,32 @@
       <c r="Y13" s="159"/>
     </row>
     <row r="14" spans="2:25" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="203" t="s">
+      <c r="B14" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="204"/>
-      <c r="D14" s="204"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="204"/>
-      <c r="G14" s="204"/>
-      <c r="H14" s="204"/>
-      <c r="I14" s="204"/>
-      <c r="J14" s="204"/>
-      <c r="K14" s="204"/>
-      <c r="L14" s="204"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="204"/>
-      <c r="O14" s="204"/>
-      <c r="P14" s="204"/>
-      <c r="Q14" s="204"/>
-      <c r="R14" s="204"/>
-      <c r="S14" s="204"/>
-      <c r="T14" s="204"/>
-      <c r="U14" s="204"/>
-      <c r="V14" s="204"/>
-      <c r="W14" s="204"/>
-      <c r="X14" s="204"/>
-      <c r="Y14" s="205"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="202"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+      <c r="Q14" s="202"/>
+      <c r="R14" s="202"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
+      <c r="U14" s="202"/>
+      <c r="V14" s="202"/>
+      <c r="W14" s="202"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="203"/>
     </row>
     <row r="15" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
@@ -14133,117 +14124,114 @@
       <c r="Y16" s="180"/>
     </row>
     <row r="17" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="216"/>
-      <c r="C17" s="216"/>
-      <c r="D17" s="216"/>
-      <c r="E17" s="216"/>
-      <c r="F17" s="216"/>
-      <c r="G17" s="216"/>
-      <c r="H17" s="216"/>
-      <c r="I17" s="216"/>
-      <c r="J17" s="216"/>
-      <c r="K17" s="216"/>
-      <c r="L17" s="216"/>
-      <c r="M17" s="216"/>
-      <c r="N17" s="216"/>
-      <c r="O17" s="216"/>
-      <c r="P17" s="216"/>
-      <c r="Q17" s="216"/>
-      <c r="R17" s="216"/>
-      <c r="S17" s="216"/>
-      <c r="T17" s="216"/>
-      <c r="U17" s="216"/>
-      <c r="V17" s="216"/>
-      <c r="W17" s="216"/>
-      <c r="X17" s="216"/>
-      <c r="Y17" s="216"/>
+      <c r="B17" s="217"/>
+      <c r="C17" s="217"/>
+      <c r="D17" s="217"/>
+      <c r="E17" s="217"/>
+      <c r="F17" s="217"/>
+      <c r="G17" s="217"/>
+      <c r="H17" s="217"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="217"/>
+      <c r="K17" s="217"/>
+      <c r="L17" s="217"/>
+      <c r="M17" s="217"/>
+      <c r="N17" s="217"/>
+      <c r="O17" s="217"/>
+      <c r="P17" s="217"/>
+      <c r="Q17" s="217"/>
+      <c r="R17" s="217"/>
+      <c r="S17" s="217"/>
+      <c r="T17" s="217"/>
+      <c r="U17" s="217"/>
+      <c r="V17" s="217"/>
+      <c r="W17" s="217"/>
+      <c r="X17" s="217"/>
+      <c r="Y17" s="217"/>
     </row>
     <row r="18" spans="2:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="198" t="e">
-        <f>Подпись.Должность</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C18" s="198"/>
-      <c r="D18" s="198"/>
-      <c r="E18" s="198"/>
-      <c r="F18" s="198"/>
-      <c r="G18" s="198"/>
-      <c r="H18" s="198"/>
-      <c r="I18" s="198"/>
-      <c r="J18" s="198"/>
-      <c r="K18" s="198"/>
-      <c r="L18" s="198"/>
-      <c r="M18" s="198"/>
-      <c r="N18" s="198"/>
-      <c r="O18" s="198"/>
-      <c r="P18" s="198"/>
-      <c r="Q18" s="198"/>
-      <c r="R18" s="198"/>
-      <c r="S18" s="198"/>
-      <c r="T18" s="198"/>
-      <c r="U18" s="198"/>
-      <c r="V18" s="198"/>
-      <c r="W18" s="198"/>
-      <c r="X18" s="198"/>
-      <c r="Y18" s="198"/>
+      <c r="B18" s="199" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="199"/>
+      <c r="D18" s="199"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
+      <c r="G18" s="199"/>
+      <c r="H18" s="199"/>
+      <c r="I18" s="199"/>
+      <c r="J18" s="199"/>
+      <c r="K18" s="199"/>
+      <c r="L18" s="199"/>
+      <c r="M18" s="199"/>
+      <c r="N18" s="199"/>
+      <c r="O18" s="199"/>
+      <c r="P18" s="199"/>
+      <c r="Q18" s="199"/>
+      <c r="R18" s="199"/>
+      <c r="S18" s="199"/>
+      <c r="T18" s="199"/>
+      <c r="U18" s="199"/>
+      <c r="V18" s="199"/>
+      <c r="W18" s="199"/>
+      <c r="X18" s="199"/>
+      <c r="Y18" s="199"/>
     </row>
     <row r="19" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="199" t="e">
-        <f>Подпись.Звание</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C19" s="199"/>
-      <c r="D19" s="199"/>
-      <c r="E19" s="199"/>
-      <c r="F19" s="199"/>
-      <c r="G19" s="199"/>
-      <c r="H19" s="199"/>
-      <c r="I19" s="199"/>
-      <c r="J19" s="199"/>
-      <c r="K19" s="199"/>
-      <c r="L19" s="199"/>
-      <c r="M19" s="199"/>
-      <c r="N19" s="199"/>
-      <c r="O19" s="199"/>
-      <c r="P19" s="199"/>
-      <c r="Q19" s="199"/>
-      <c r="R19" s="199"/>
-      <c r="S19" s="199"/>
-      <c r="T19" s="199"/>
-      <c r="U19" s="199"/>
-      <c r="V19" s="199"/>
-      <c r="W19" s="199"/>
-      <c r="X19" s="199"/>
-      <c r="Y19" s="199"/>
+      <c r="B19" s="200" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="200"/>
+      <c r="D19" s="200"/>
+      <c r="E19" s="200"/>
+      <c r="F19" s="200"/>
+      <c r="G19" s="200"/>
+      <c r="H19" s="200"/>
+      <c r="I19" s="200"/>
+      <c r="J19" s="200"/>
+      <c r="K19" s="200"/>
+      <c r="L19" s="200"/>
+      <c r="M19" s="200"/>
+      <c r="N19" s="200"/>
+      <c r="O19" s="200"/>
+      <c r="P19" s="200"/>
+      <c r="Q19" s="200"/>
+      <c r="R19" s="200"/>
+      <c r="S19" s="200"/>
+      <c r="T19" s="200"/>
+      <c r="U19" s="200"/>
+      <c r="V19" s="200"/>
+      <c r="W19" s="200"/>
+      <c r="X19" s="200"/>
+      <c r="Y19" s="200"/>
     </row>
     <row r="20" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="194" t="e">
-        <f>Подпись.ИФамилия</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C20" s="194"/>
-      <c r="D20" s="194"/>
-      <c r="E20" s="194"/>
-      <c r="F20" s="194"/>
-      <c r="G20" s="194"/>
-      <c r="H20" s="194"/>
-      <c r="I20" s="194"/>
-      <c r="J20" s="194"/>
-      <c r="K20" s="194"/>
-      <c r="L20" s="194"/>
-      <c r="M20" s="194"/>
-      <c r="N20" s="194"/>
-      <c r="O20" s="194"/>
-      <c r="P20" s="194"/>
-      <c r="Q20" s="194"/>
-      <c r="R20" s="194"/>
-      <c r="S20" s="194"/>
-      <c r="T20" s="194"/>
-      <c r="U20" s="194"/>
-      <c r="V20" s="194"/>
-      <c r="W20" s="194"/>
-      <c r="X20" s="194"/>
-      <c r="Y20" s="194"/>
+      <c r="B20" s="195" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="195"/>
+      <c r="D20" s="195"/>
+      <c r="E20" s="195"/>
+      <c r="F20" s="195"/>
+      <c r="G20" s="195"/>
+      <c r="H20" s="195"/>
+      <c r="I20" s="195"/>
+      <c r="J20" s="195"/>
+      <c r="K20" s="195"/>
+      <c r="L20" s="195"/>
+      <c r="M20" s="195"/>
+      <c r="N20" s="195"/>
+      <c r="O20" s="195"/>
+      <c r="P20" s="195"/>
+      <c r="Q20" s="195"/>
+      <c r="R20" s="195"/>
+      <c r="S20" s="195"/>
+      <c r="T20" s="195"/>
+      <c r="U20" s="195"/>
+      <c r="V20" s="195"/>
+      <c r="W20" s="195"/>
+      <c r="X20" s="195"/>
+      <c r="Y20" s="195"/>
     </row>
     <row r="21" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X21" s="108"/>
@@ -17037,108 +17025,108 @@
       <c r="X950" s="108"/>
     </row>
     <row r="951" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B951" s="213"/>
-      <c r="C951" s="213"/>
-      <c r="D951" s="213"/>
-      <c r="E951" s="213"/>
-      <c r="F951" s="213"/>
-      <c r="G951" s="213"/>
-      <c r="H951" s="213"/>
-      <c r="I951" s="213"/>
-      <c r="J951" s="213"/>
-      <c r="K951" s="213"/>
-      <c r="L951" s="213"/>
-      <c r="M951" s="213"/>
-      <c r="N951" s="213"/>
-      <c r="O951" s="213"/>
-      <c r="P951" s="213"/>
-      <c r="Q951" s="213"/>
-      <c r="R951" s="213"/>
-      <c r="S951" s="213"/>
-      <c r="T951" s="213"/>
-      <c r="U951" s="213"/>
-      <c r="V951" s="213"/>
-      <c r="W951" s="213"/>
-      <c r="X951" s="213"/>
-      <c r="Y951" s="213"/>
+      <c r="B951" s="214"/>
+      <c r="C951" s="214"/>
+      <c r="D951" s="214"/>
+      <c r="E951" s="214"/>
+      <c r="F951" s="214"/>
+      <c r="G951" s="214"/>
+      <c r="H951" s="214"/>
+      <c r="I951" s="214"/>
+      <c r="J951" s="214"/>
+      <c r="K951" s="214"/>
+      <c r="L951" s="214"/>
+      <c r="M951" s="214"/>
+      <c r="N951" s="214"/>
+      <c r="O951" s="214"/>
+      <c r="P951" s="214"/>
+      <c r="Q951" s="214"/>
+      <c r="R951" s="214"/>
+      <c r="S951" s="214"/>
+      <c r="T951" s="214"/>
+      <c r="U951" s="214"/>
+      <c r="V951" s="214"/>
+      <c r="W951" s="214"/>
+      <c r="X951" s="214"/>
+      <c r="Y951" s="214"/>
     </row>
     <row r="952" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B952" s="214"/>
-      <c r="C952" s="214"/>
-      <c r="D952" s="214"/>
-      <c r="E952" s="214"/>
-      <c r="F952" s="214"/>
-      <c r="G952" s="214"/>
-      <c r="H952" s="214"/>
-      <c r="I952" s="214"/>
-      <c r="J952" s="214"/>
-      <c r="K952" s="214"/>
-      <c r="L952" s="214"/>
-      <c r="M952" s="214"/>
-      <c r="N952" s="214"/>
-      <c r="O952" s="214"/>
-      <c r="P952" s="214"/>
-      <c r="Q952" s="214"/>
-      <c r="R952" s="214"/>
-      <c r="S952" s="214"/>
-      <c r="T952" s="214"/>
-      <c r="U952" s="214"/>
-      <c r="V952" s="214"/>
-      <c r="W952" s="214"/>
-      <c r="X952" s="214"/>
-      <c r="Y952" s="214"/>
+      <c r="B952" s="215"/>
+      <c r="C952" s="215"/>
+      <c r="D952" s="215"/>
+      <c r="E952" s="215"/>
+      <c r="F952" s="215"/>
+      <c r="G952" s="215"/>
+      <c r="H952" s="215"/>
+      <c r="I952" s="215"/>
+      <c r="J952" s="215"/>
+      <c r="K952" s="215"/>
+      <c r="L952" s="215"/>
+      <c r="M952" s="215"/>
+      <c r="N952" s="215"/>
+      <c r="O952" s="215"/>
+      <c r="P952" s="215"/>
+      <c r="Q952" s="215"/>
+      <c r="R952" s="215"/>
+      <c r="S952" s="215"/>
+      <c r="T952" s="215"/>
+      <c r="U952" s="215"/>
+      <c r="V952" s="215"/>
+      <c r="W952" s="215"/>
+      <c r="X952" s="215"/>
+      <c r="Y952" s="215"/>
     </row>
     <row r="953" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B953" s="215"/>
-      <c r="C953" s="215"/>
-      <c r="D953" s="215"/>
-      <c r="E953" s="215"/>
-      <c r="F953" s="215"/>
-      <c r="G953" s="215"/>
-      <c r="H953" s="215"/>
-      <c r="I953" s="215"/>
-      <c r="J953" s="215"/>
-      <c r="K953" s="215"/>
-      <c r="L953" s="215"/>
-      <c r="M953" s="215"/>
-      <c r="N953" s="215"/>
-      <c r="O953" s="215"/>
-      <c r="P953" s="215"/>
-      <c r="Q953" s="215"/>
-      <c r="R953" s="215"/>
-      <c r="S953" s="215"/>
-      <c r="T953" s="215"/>
-      <c r="U953" s="215"/>
-      <c r="V953" s="215"/>
-      <c r="W953" s="215"/>
-      <c r="X953" s="215"/>
-      <c r="Y953" s="215"/>
+      <c r="B953" s="216"/>
+      <c r="C953" s="216"/>
+      <c r="D953" s="216"/>
+      <c r="E953" s="216"/>
+      <c r="F953" s="216"/>
+      <c r="G953" s="216"/>
+      <c r="H953" s="216"/>
+      <c r="I953" s="216"/>
+      <c r="J953" s="216"/>
+      <c r="K953" s="216"/>
+      <c r="L953" s="216"/>
+      <c r="M953" s="216"/>
+      <c r="N953" s="216"/>
+      <c r="O953" s="216"/>
+      <c r="P953" s="216"/>
+      <c r="Q953" s="216"/>
+      <c r="R953" s="216"/>
+      <c r="S953" s="216"/>
+      <c r="T953" s="216"/>
+      <c r="U953" s="216"/>
+      <c r="V953" s="216"/>
+      <c r="W953" s="216"/>
+      <c r="X953" s="216"/>
+      <c r="Y953" s="216"/>
     </row>
     <row r="954" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B954" s="212"/>
-      <c r="C954" s="212"/>
-      <c r="D954" s="212"/>
-      <c r="E954" s="212"/>
-      <c r="F954" s="212"/>
-      <c r="G954" s="212"/>
-      <c r="H954" s="212"/>
-      <c r="I954" s="212"/>
-      <c r="J954" s="212"/>
-      <c r="K954" s="212"/>
-      <c r="L954" s="212"/>
-      <c r="M954" s="212"/>
-      <c r="N954" s="212"/>
-      <c r="O954" s="212"/>
-      <c r="P954" s="212"/>
-      <c r="Q954" s="212"/>
-      <c r="R954" s="212"/>
-      <c r="S954" s="212"/>
-      <c r="T954" s="212"/>
-      <c r="U954" s="212"/>
-      <c r="V954" s="212"/>
-      <c r="W954" s="212"/>
-      <c r="X954" s="212"/>
-      <c r="Y954" s="212"/>
+      <c r="B954" s="213"/>
+      <c r="C954" s="213"/>
+      <c r="D954" s="213"/>
+      <c r="E954" s="213"/>
+      <c r="F954" s="213"/>
+      <c r="G954" s="213"/>
+      <c r="H954" s="213"/>
+      <c r="I954" s="213"/>
+      <c r="J954" s="213"/>
+      <c r="K954" s="213"/>
+      <c r="L954" s="213"/>
+      <c r="M954" s="213"/>
+      <c r="N954" s="213"/>
+      <c r="O954" s="213"/>
+      <c r="P954" s="213"/>
+      <c r="Q954" s="213"/>
+      <c r="R954" s="213"/>
+      <c r="S954" s="213"/>
+      <c r="T954" s="213"/>
+      <c r="U954" s="213"/>
+      <c r="V954" s="213"/>
+      <c r="W954" s="213"/>
+      <c r="X954" s="213"/>
+      <c r="Y954" s="213"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
@@ -17220,118 +17208,118 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:111" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="217" t="e">
+      <c r="A2" s="218" t="e">
         <f>CONCATENATE("Ведомость результатов подготовки курсантов ",'1б'!#REF!," учебного взвода за ",'1б'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="217"/>
-      <c r="J2" s="217"/>
-      <c r="K2" s="217"/>
-      <c r="L2" s="217"/>
-      <c r="M2" s="217"/>
-      <c r="N2" s="217"/>
-      <c r="O2" s="217"/>
-      <c r="P2" s="217"/>
-      <c r="Q2" s="217"/>
-      <c r="R2" s="217"/>
-      <c r="S2" s="217"/>
-      <c r="T2" s="217"/>
-      <c r="U2" s="217"/>
-      <c r="V2" s="217"/>
-      <c r="W2" s="217"/>
-      <c r="X2" s="217"/>
-      <c r="Y2" s="217"/>
-      <c r="Z2" s="217"/>
-      <c r="AA2" s="217"/>
-      <c r="AB2" s="217"/>
-      <c r="AC2" s="217"/>
-      <c r="AD2" s="217"/>
-      <c r="AE2" s="217"/>
-      <c r="AF2" s="217"/>
-      <c r="AG2" s="217"/>
-      <c r="AH2" s="217"/>
-      <c r="AI2" s="217"/>
-      <c r="AJ2" s="217"/>
-      <c r="AK2" s="217"/>
-      <c r="AL2" s="217"/>
-      <c r="AM2" s="217"/>
-      <c r="AN2" s="217"/>
-      <c r="AO2" s="217"/>
-      <c r="AP2" s="217"/>
-      <c r="AQ2" s="217"/>
-      <c r="AR2" s="217"/>
-      <c r="AS2" s="217"/>
-      <c r="AT2" s="217"/>
-      <c r="AU2" s="217"/>
-      <c r="AV2" s="217"/>
-      <c r="AW2" s="217"/>
-      <c r="AX2" s="217"/>
-      <c r="AY2" s="217"/>
-      <c r="AZ2" s="217"/>
-      <c r="BA2" s="217"/>
-      <c r="BB2" s="217"/>
-      <c r="BC2" s="217"/>
-      <c r="BD2" s="217"/>
-      <c r="BE2" s="217"/>
-      <c r="BF2" s="217"/>
-      <c r="BG2" s="217"/>
-      <c r="BH2" s="217"/>
-      <c r="BI2" s="217"/>
-      <c r="BJ2" s="217"/>
-      <c r="BK2" s="217"/>
-      <c r="BL2" s="217"/>
-      <c r="BM2" s="217"/>
-      <c r="BN2" s="217"/>
-      <c r="BO2" s="217"/>
-      <c r="BP2" s="217"/>
-      <c r="BQ2" s="217"/>
-      <c r="BR2" s="217"/>
-      <c r="BS2" s="217"/>
-      <c r="BT2" s="217"/>
-      <c r="BU2" s="217"/>
-      <c r="BV2" s="217"/>
-      <c r="BW2" s="217"/>
-      <c r="BX2" s="217"/>
-      <c r="BY2" s="217"/>
-      <c r="BZ2" s="217"/>
-      <c r="CA2" s="217"/>
-      <c r="CB2" s="217"/>
-      <c r="CC2" s="217"/>
-      <c r="CD2" s="217"/>
-      <c r="CE2" s="217"/>
-      <c r="CF2" s="217"/>
-      <c r="CG2" s="217"/>
-      <c r="CH2" s="217"/>
-      <c r="CI2" s="217"/>
-      <c r="CJ2" s="217"/>
-      <c r="CK2" s="217"/>
-      <c r="CL2" s="217"/>
-      <c r="CM2" s="217"/>
-      <c r="CN2" s="217"/>
-      <c r="CO2" s="217"/>
-      <c r="CP2" s="217"/>
-      <c r="CQ2" s="217"/>
-      <c r="CR2" s="217"/>
-      <c r="CS2" s="217"/>
-      <c r="CT2" s="217"/>
-      <c r="CU2" s="217"/>
-      <c r="CV2" s="217"/>
-      <c r="CW2" s="217"/>
-      <c r="CX2" s="217"/>
-      <c r="CY2" s="217"/>
-      <c r="CZ2" s="217"/>
-      <c r="DA2" s="217"/>
-      <c r="DB2" s="217"/>
-      <c r="DC2" s="217"/>
-      <c r="DD2" s="217"/>
-      <c r="DE2" s="217"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
+      <c r="J2" s="218"/>
+      <c r="K2" s="218"/>
+      <c r="L2" s="218"/>
+      <c r="M2" s="218"/>
+      <c r="N2" s="218"/>
+      <c r="O2" s="218"/>
+      <c r="P2" s="218"/>
+      <c r="Q2" s="218"/>
+      <c r="R2" s="218"/>
+      <c r="S2" s="218"/>
+      <c r="T2" s="218"/>
+      <c r="U2" s="218"/>
+      <c r="V2" s="218"/>
+      <c r="W2" s="218"/>
+      <c r="X2" s="218"/>
+      <c r="Y2" s="218"/>
+      <c r="Z2" s="218"/>
+      <c r="AA2" s="218"/>
+      <c r="AB2" s="218"/>
+      <c r="AC2" s="218"/>
+      <c r="AD2" s="218"/>
+      <c r="AE2" s="218"/>
+      <c r="AF2" s="218"/>
+      <c r="AG2" s="218"/>
+      <c r="AH2" s="218"/>
+      <c r="AI2" s="218"/>
+      <c r="AJ2" s="218"/>
+      <c r="AK2" s="218"/>
+      <c r="AL2" s="218"/>
+      <c r="AM2" s="218"/>
+      <c r="AN2" s="218"/>
+      <c r="AO2" s="218"/>
+      <c r="AP2" s="218"/>
+      <c r="AQ2" s="218"/>
+      <c r="AR2" s="218"/>
+      <c r="AS2" s="218"/>
+      <c r="AT2" s="218"/>
+      <c r="AU2" s="218"/>
+      <c r="AV2" s="218"/>
+      <c r="AW2" s="218"/>
+      <c r="AX2" s="218"/>
+      <c r="AY2" s="218"/>
+      <c r="AZ2" s="218"/>
+      <c r="BA2" s="218"/>
+      <c r="BB2" s="218"/>
+      <c r="BC2" s="218"/>
+      <c r="BD2" s="218"/>
+      <c r="BE2" s="218"/>
+      <c r="BF2" s="218"/>
+      <c r="BG2" s="218"/>
+      <c r="BH2" s="218"/>
+      <c r="BI2" s="218"/>
+      <c r="BJ2" s="218"/>
+      <c r="BK2" s="218"/>
+      <c r="BL2" s="218"/>
+      <c r="BM2" s="218"/>
+      <c r="BN2" s="218"/>
+      <c r="BO2" s="218"/>
+      <c r="BP2" s="218"/>
+      <c r="BQ2" s="218"/>
+      <c r="BR2" s="218"/>
+      <c r="BS2" s="218"/>
+      <c r="BT2" s="218"/>
+      <c r="BU2" s="218"/>
+      <c r="BV2" s="218"/>
+      <c r="BW2" s="218"/>
+      <c r="BX2" s="218"/>
+      <c r="BY2" s="218"/>
+      <c r="BZ2" s="218"/>
+      <c r="CA2" s="218"/>
+      <c r="CB2" s="218"/>
+      <c r="CC2" s="218"/>
+      <c r="CD2" s="218"/>
+      <c r="CE2" s="218"/>
+      <c r="CF2" s="218"/>
+      <c r="CG2" s="218"/>
+      <c r="CH2" s="218"/>
+      <c r="CI2" s="218"/>
+      <c r="CJ2" s="218"/>
+      <c r="CK2" s="218"/>
+      <c r="CL2" s="218"/>
+      <c r="CM2" s="218"/>
+      <c r="CN2" s="218"/>
+      <c r="CO2" s="218"/>
+      <c r="CP2" s="218"/>
+      <c r="CQ2" s="218"/>
+      <c r="CR2" s="218"/>
+      <c r="CS2" s="218"/>
+      <c r="CT2" s="218"/>
+      <c r="CU2" s="218"/>
+      <c r="CV2" s="218"/>
+      <c r="CW2" s="218"/>
+      <c r="CX2" s="218"/>
+      <c r="CY2" s="218"/>
+      <c r="CZ2" s="218"/>
+      <c r="DA2" s="218"/>
+      <c r="DB2" s="218"/>
+      <c r="DC2" s="218"/>
+      <c r="DD2" s="218"/>
+      <c r="DE2" s="218"/>
     </row>
     <row r="4" spans="1:111" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
@@ -35266,13 +35254,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId2"/>
@@ -35284,13 +35272,13 @@
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId5"/>

</xml_diff>

<commit_message>
tweaked officer grade list template
</commit_message>
<xml_diff>
--- a/templates/список_оценок_контрактники.xlsx
+++ b/templates/список_оценок_контрактники.xlsx
@@ -180,13 +180,13 @@
     <definedName name="Подпись.Звание">Главная!#REF!</definedName>
     <definedName name="Подпись.ИФамилия">Главная!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Admin - Личное представление" guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="767" tabRatio="919" activeSheetId="2"/>
+    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
+    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
+    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
     <customWorkbookView name="Огнедышащий воробей - Личное представление" guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="548" tabRatio="919" activeSheetId="8"/>
-    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
-    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
-    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
-    <customWorkbookView name="Admin - Личное представление" guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="767" tabRatio="919" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1700,15 +1700,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1718,6 +1718,10 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1732,20 +1736,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1762,10 +1766,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2236,17 +2236,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="85" showPageBreaks="1" printArea="1">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="85" showPageBreaks="1" printArea="1">
       <pane xSplit="30" ySplit="28" topLeftCell="AE29" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="85" showPageBreaks="1" printArea="1">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="85" showPageBreaks="1" printArea="1">
       <pane xSplit="30" ySplit="28" topLeftCell="AE29" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="C4" s="217"/>
       <c r="D4" s="217"/>
-      <c r="E4" s="214"/>
+      <c r="E4" s="218"/>
       <c r="F4" s="217"/>
       <c r="G4" s="217"/>
       <c r="H4" s="217"/>
@@ -2976,7 +2976,7 @@
       <c r="V4" s="217"/>
       <c r="W4" s="217"/>
       <c r="X4" s="217"/>
-      <c r="Y4" s="218"/>
+      <c r="Y4" s="219"/>
     </row>
     <row r="5" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="137"/>
@@ -3193,7 +3193,7 @@
       <c r="V11" s="217"/>
       <c r="W11" s="217"/>
       <c r="X11" s="217"/>
-      <c r="Y11" s="218"/>
+      <c r="Y11" s="219"/>
     </row>
     <row r="12" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C18" s="217"/>
       <c r="D18" s="217"/>
-      <c r="E18" s="214"/>
+      <c r="E18" s="218"/>
       <c r="F18" s="217"/>
       <c r="G18" s="217"/>
       <c r="H18" s="217"/>
@@ -3409,7 +3409,7 @@
       <c r="V18" s="217"/>
       <c r="W18" s="217"/>
       <c r="X18" s="217"/>
-      <c r="Y18" s="218"/>
+      <c r="Y18" s="219"/>
     </row>
     <row r="19" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="C25" s="217"/>
       <c r="D25" s="217"/>
-      <c r="E25" s="214"/>
+      <c r="E25" s="218"/>
       <c r="F25" s="217"/>
       <c r="G25" s="217"/>
       <c r="H25" s="217"/>
@@ -3645,7 +3645,7 @@
       <c r="V25" s="217"/>
       <c r="W25" s="217"/>
       <c r="X25" s="217"/>
-      <c r="Y25" s="218"/>
+      <c r="Y25" s="219"/>
     </row>
     <row r="26" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="141" t="s">
@@ -3832,58 +3832,58 @@
       <c r="Y30" s="117"/>
     </row>
     <row r="31" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="219"/>
-      <c r="C31" s="219"/>
-      <c r="D31" s="219"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="219"/>
-      <c r="G31" s="219"/>
-      <c r="H31" s="219"/>
-      <c r="I31" s="219"/>
-      <c r="J31" s="219"/>
-      <c r="K31" s="219"/>
-      <c r="L31" s="219"/>
-      <c r="M31" s="219"/>
-      <c r="N31" s="219"/>
-      <c r="O31" s="219"/>
-      <c r="P31" s="219"/>
-      <c r="Q31" s="219"/>
-      <c r="R31" s="219"/>
-      <c r="S31" s="219"/>
-      <c r="T31" s="219"/>
-      <c r="U31" s="219"/>
-      <c r="V31" s="219"/>
-      <c r="W31" s="219"/>
-      <c r="X31" s="219"/>
-      <c r="Y31" s="219"/>
+      <c r="B31" s="220"/>
+      <c r="C31" s="220"/>
+      <c r="D31" s="220"/>
+      <c r="E31" s="221"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
+      <c r="M31" s="220"/>
+      <c r="N31" s="220"/>
+      <c r="O31" s="220"/>
+      <c r="P31" s="220"/>
+      <c r="Q31" s="220"/>
+      <c r="R31" s="220"/>
+      <c r="S31" s="220"/>
+      <c r="T31" s="220"/>
+      <c r="U31" s="220"/>
+      <c r="V31" s="220"/>
+      <c r="W31" s="220"/>
+      <c r="X31" s="220"/>
+      <c r="Y31" s="220"/>
     </row>
     <row r="32" spans="2:26" s="110" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="213" t="s">
+      <c r="B32" s="222" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="214"/>
-      <c r="D32" s="214"/>
-      <c r="E32" s="214"/>
-      <c r="F32" s="214"/>
-      <c r="G32" s="214"/>
-      <c r="H32" s="214"/>
-      <c r="I32" s="214"/>
-      <c r="J32" s="214"/>
-      <c r="K32" s="214"/>
-      <c r="L32" s="214"/>
-      <c r="M32" s="214"/>
-      <c r="N32" s="214"/>
-      <c r="O32" s="214"/>
-      <c r="P32" s="214"/>
-      <c r="Q32" s="214"/>
-      <c r="R32" s="214"/>
-      <c r="S32" s="214"/>
-      <c r="T32" s="214"/>
-      <c r="U32" s="214"/>
-      <c r="V32" s="214"/>
-      <c r="W32" s="214"/>
-      <c r="X32" s="214"/>
-      <c r="Y32" s="215"/>
+      <c r="C32" s="218"/>
+      <c r="D32" s="218"/>
+      <c r="E32" s="218"/>
+      <c r="F32" s="218"/>
+      <c r="G32" s="218"/>
+      <c r="H32" s="218"/>
+      <c r="I32" s="218"/>
+      <c r="J32" s="218"/>
+      <c r="K32" s="218"/>
+      <c r="L32" s="218"/>
+      <c r="M32" s="218"/>
+      <c r="N32" s="218"/>
+      <c r="O32" s="218"/>
+      <c r="P32" s="218"/>
+      <c r="Q32" s="218"/>
+      <c r="R32" s="218"/>
+      <c r="S32" s="218"/>
+      <c r="T32" s="218"/>
+      <c r="U32" s="218"/>
+      <c r="V32" s="218"/>
+      <c r="W32" s="218"/>
+      <c r="X32" s="218"/>
+      <c r="Y32" s="223"/>
     </row>
     <row r="33" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="141" t="s">
@@ -4094,32 +4094,32 @@
       <c r="X38" s="118"/>
     </row>
     <row r="39" spans="2:26" s="110" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="221" t="s">
+      <c r="B39" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="222"/>
-      <c r="D39" s="222"/>
-      <c r="E39" s="222"/>
-      <c r="F39" s="222"/>
-      <c r="G39" s="222"/>
-      <c r="H39" s="222"/>
-      <c r="I39" s="222"/>
-      <c r="J39" s="222"/>
-      <c r="K39" s="222"/>
-      <c r="L39" s="222"/>
-      <c r="M39" s="222"/>
-      <c r="N39" s="222"/>
-      <c r="O39" s="222"/>
-      <c r="P39" s="222"/>
-      <c r="Q39" s="222"/>
-      <c r="R39" s="222"/>
-      <c r="S39" s="222"/>
-      <c r="T39" s="222"/>
-      <c r="U39" s="222"/>
-      <c r="V39" s="222"/>
-      <c r="W39" s="222"/>
-      <c r="X39" s="222"/>
-      <c r="Y39" s="223"/>
+      <c r="C39" s="214"/>
+      <c r="D39" s="214"/>
+      <c r="E39" s="214"/>
+      <c r="F39" s="214"/>
+      <c r="G39" s="214"/>
+      <c r="H39" s="214"/>
+      <c r="I39" s="214"/>
+      <c r="J39" s="214"/>
+      <c r="K39" s="214"/>
+      <c r="L39" s="214"/>
+      <c r="M39" s="214"/>
+      <c r="N39" s="214"/>
+      <c r="O39" s="214"/>
+      <c r="P39" s="214"/>
+      <c r="Q39" s="214"/>
+      <c r="R39" s="214"/>
+      <c r="S39" s="214"/>
+      <c r="T39" s="214"/>
+      <c r="U39" s="214"/>
+      <c r="V39" s="214"/>
+      <c r="W39" s="214"/>
+      <c r="X39" s="214"/>
+      <c r="Y39" s="215"/>
     </row>
     <row r="40" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="141" t="s">
@@ -4480,11 +4480,11 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="25">
-    <mergeCell ref="B48:Y48"/>
-    <mergeCell ref="B47:Y47"/>
-    <mergeCell ref="B46:Y46"/>
-    <mergeCell ref="B45:Y45"/>
-    <mergeCell ref="B39:Y39"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B32:Y32"/>
     <mergeCell ref="B3:Y3"/>
     <mergeCell ref="B4:Y4"/>
     <mergeCell ref="B2:Y2"/>
@@ -4500,11 +4500,11 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B32:Y32"/>
+    <mergeCell ref="B48:Y48"/>
+    <mergeCell ref="B47:Y47"/>
+    <mergeCell ref="B46:Y46"/>
+    <mergeCell ref="B45:Y45"/>
+    <mergeCell ref="B39:Y39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.69" bottom="0.27" header="0.84" footer="0.28999999999999998"/>
@@ -4674,32 +4674,32 @@
       <c r="Y3" s="206"/>
     </row>
     <row r="4" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="222" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="214"/>
-      <c r="M4" s="214"/>
-      <c r="N4" s="214"/>
-      <c r="O4" s="214"/>
-      <c r="P4" s="214"/>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="214"/>
-      <c r="S4" s="214"/>
-      <c r="T4" s="214"/>
-      <c r="U4" s="214"/>
-      <c r="V4" s="214"/>
-      <c r="W4" s="214"/>
-      <c r="X4" s="214"/>
-      <c r="Y4" s="215"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="218"/>
+      <c r="K4" s="218"/>
+      <c r="L4" s="218"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="218"/>
+      <c r="Q4" s="218"/>
+      <c r="R4" s="218"/>
+      <c r="S4" s="218"/>
+      <c r="T4" s="218"/>
+      <c r="U4" s="218"/>
+      <c r="V4" s="218"/>
+      <c r="W4" s="218"/>
+      <c r="X4" s="218"/>
+      <c r="Y4" s="223"/>
     </row>
     <row r="5" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -4912,32 +4912,32 @@
       <c r="Y10" s="156"/>
     </row>
     <row r="11" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="222" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="214"/>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="214"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="214"/>
-      <c r="M11" s="214"/>
-      <c r="N11" s="214"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="214"/>
-      <c r="Q11" s="214"/>
-      <c r="R11" s="214"/>
-      <c r="S11" s="214"/>
-      <c r="T11" s="214"/>
-      <c r="U11" s="214"/>
-      <c r="V11" s="214"/>
-      <c r="W11" s="214"/>
-      <c r="X11" s="214"/>
-      <c r="Y11" s="215"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="218"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="218"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="218"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="218"/>
+      <c r="U11" s="218"/>
+      <c r="V11" s="218"/>
+      <c r="W11" s="218"/>
+      <c r="X11" s="218"/>
+      <c r="Y11" s="223"/>
     </row>
     <row r="12" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
@@ -5150,32 +5150,32 @@
       <c r="Y17" s="159"/>
     </row>
     <row r="18" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="213" t="s">
+      <c r="B18" s="222" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="214"/>
-      <c r="O18" s="214"/>
-      <c r="P18" s="214"/>
-      <c r="Q18" s="214"/>
-      <c r="R18" s="214"/>
-      <c r="S18" s="214"/>
-      <c r="T18" s="214"/>
-      <c r="U18" s="214"/>
-      <c r="V18" s="214"/>
-      <c r="W18" s="214"/>
-      <c r="X18" s="214"/>
-      <c r="Y18" s="215"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="218"/>
+      <c r="E18" s="218"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="218"/>
+      <c r="M18" s="218"/>
+      <c r="N18" s="218"/>
+      <c r="O18" s="218"/>
+      <c r="P18" s="218"/>
+      <c r="Q18" s="218"/>
+      <c r="R18" s="218"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
+      <c r="V18" s="218"/>
+      <c r="W18" s="218"/>
+      <c r="X18" s="218"/>
+      <c r="Y18" s="223"/>
     </row>
     <row r="19" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
@@ -5388,32 +5388,32 @@
       <c r="Y24" s="137"/>
     </row>
     <row r="25" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="213" t="s">
+      <c r="B25" s="222" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="214"/>
-      <c r="D25" s="214"/>
-      <c r="E25" s="214"/>
-      <c r="F25" s="214"/>
-      <c r="G25" s="214"/>
-      <c r="H25" s="214"/>
-      <c r="I25" s="214"/>
-      <c r="J25" s="214"/>
-      <c r="K25" s="214"/>
-      <c r="L25" s="214"/>
-      <c r="M25" s="214"/>
-      <c r="N25" s="214"/>
-      <c r="O25" s="214"/>
-      <c r="P25" s="214"/>
-      <c r="Q25" s="214"/>
-      <c r="R25" s="214"/>
-      <c r="S25" s="214"/>
-      <c r="T25" s="214"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="214"/>
-      <c r="W25" s="214"/>
-      <c r="X25" s="214"/>
-      <c r="Y25" s="215"/>
+      <c r="C25" s="218"/>
+      <c r="D25" s="218"/>
+      <c r="E25" s="218"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="218"/>
+      <c r="H25" s="218"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="218"/>
+      <c r="L25" s="218"/>
+      <c r="M25" s="218"/>
+      <c r="N25" s="218"/>
+      <c r="O25" s="218"/>
+      <c r="P25" s="218"/>
+      <c r="Q25" s="218"/>
+      <c r="R25" s="218"/>
+      <c r="S25" s="218"/>
+      <c r="T25" s="218"/>
+      <c r="U25" s="218"/>
+      <c r="V25" s="218"/>
+      <c r="W25" s="218"/>
+      <c r="X25" s="218"/>
+      <c r="Y25" s="223"/>
     </row>
     <row r="26" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="141" t="s">
@@ -5711,18 +5711,23 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <customSheetViews>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="26" fitToHeight="4" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" scale="85" showAutoFilter="1" hiddenColumns="1" showRuler="0" topLeftCell="A1417">
-      <selection activeCell="M1442" sqref="M1442"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="landscape" horizontalDpi="120" verticalDpi="144" r:id="rId2"/>
+    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" hiddenColumns="1" showRuler="0">
+      <pane xSplit="35.840909090909093" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G529" sqref="G529"/>
+      <colBreaks count="1" manualBreakCount="1">
+        <brk id="17" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.3" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
+      <printOptions horizontalCentered="1"/>
+      <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
@@ -5733,21 +5738,16 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
-    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" hiddenColumns="1" showRuler="0">
-      <pane xSplit="35.840909090909093" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G529" sqref="G529"/>
-      <colBreaks count="1" manualBreakCount="1">
-        <brk id="17" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.3" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
-      <printOptions horizontalCentered="1"/>
-      <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId4"/>
+    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" scale="85" showAutoFilter="1" hiddenColumns="1" showRuler="0" topLeftCell="A1417">
+      <selection activeCell="M1442" sqref="M1442"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="landscape" horizontalDpi="120" verticalDpi="144" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1"/>
     </customSheetView>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="55" showPageBreaks="1" fitToPage="1" hiddenRows="1" hiddenColumns="1" view="pageBreakPreview">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
       <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19" bottom="0.27" header="0.51181102362204722" footer="0.28999999999999998"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="26" fitToHeight="4" orientation="portrait" r:id="rId5"/>
@@ -5755,6 +5755,12 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="18">
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B32:Y32"/>
+    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="B31:Y31"/>
+    <mergeCell ref="B30:Y30"/>
     <mergeCell ref="B2:Y2"/>
     <mergeCell ref="B3:Y3"/>
     <mergeCell ref="B25:Y25"/>
@@ -5767,12 +5773,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B32:Y32"/>
-    <mergeCell ref="B33:Y33"/>
-    <mergeCell ref="B31:Y31"/>
-    <mergeCell ref="B30:Y30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -5940,32 +5940,32 @@
       <c r="Y3" s="206"/>
     </row>
     <row r="4" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="222" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="214"/>
-      <c r="M4" s="214"/>
-      <c r="N4" s="214"/>
-      <c r="O4" s="214"/>
-      <c r="P4" s="214"/>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="214"/>
-      <c r="S4" s="214"/>
-      <c r="T4" s="214"/>
-      <c r="U4" s="214"/>
-      <c r="V4" s="214"/>
-      <c r="W4" s="214"/>
-      <c r="X4" s="214"/>
-      <c r="Y4" s="215"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="218"/>
+      <c r="K4" s="218"/>
+      <c r="L4" s="218"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="218"/>
+      <c r="Q4" s="218"/>
+      <c r="R4" s="218"/>
+      <c r="S4" s="218"/>
+      <c r="T4" s="218"/>
+      <c r="U4" s="218"/>
+      <c r="V4" s="218"/>
+      <c r="W4" s="218"/>
+      <c r="X4" s="218"/>
+      <c r="Y4" s="223"/>
     </row>
     <row r="5" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -6178,32 +6178,32 @@
       <c r="Y10" s="135"/>
     </row>
     <row r="11" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="222" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="214"/>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="214"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="214"/>
-      <c r="M11" s="214"/>
-      <c r="N11" s="214"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="214"/>
-      <c r="Q11" s="214"/>
-      <c r="R11" s="214"/>
-      <c r="S11" s="214"/>
-      <c r="T11" s="214"/>
-      <c r="U11" s="214"/>
-      <c r="V11" s="214"/>
-      <c r="W11" s="214"/>
-      <c r="X11" s="214"/>
-      <c r="Y11" s="215"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="218"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="218"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="218"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="218"/>
+      <c r="U11" s="218"/>
+      <c r="V11" s="218"/>
+      <c r="W11" s="218"/>
+      <c r="X11" s="218"/>
+      <c r="Y11" s="223"/>
     </row>
     <row r="12" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
@@ -6416,32 +6416,32 @@
       <c r="Y17" s="135"/>
     </row>
     <row r="18" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="213" t="s">
+      <c r="B18" s="222" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="214"/>
-      <c r="O18" s="214"/>
-      <c r="P18" s="214"/>
-      <c r="Q18" s="214"/>
-      <c r="R18" s="214"/>
-      <c r="S18" s="214"/>
-      <c r="T18" s="214"/>
-      <c r="U18" s="214"/>
-      <c r="V18" s="214"/>
-      <c r="W18" s="214"/>
-      <c r="X18" s="214"/>
-      <c r="Y18" s="215"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="218"/>
+      <c r="E18" s="218"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="218"/>
+      <c r="M18" s="218"/>
+      <c r="N18" s="218"/>
+      <c r="O18" s="218"/>
+      <c r="P18" s="218"/>
+      <c r="Q18" s="218"/>
+      <c r="R18" s="218"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
+      <c r="V18" s="218"/>
+      <c r="W18" s="218"/>
+      <c r="X18" s="218"/>
+      <c r="Y18" s="223"/>
     </row>
     <row r="19" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
@@ -6654,32 +6654,32 @@
       <c r="Y24" s="173"/>
     </row>
     <row r="25" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="213" t="s">
+      <c r="B25" s="222" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="214"/>
-      <c r="D25" s="214"/>
-      <c r="E25" s="214"/>
-      <c r="F25" s="214"/>
-      <c r="G25" s="214"/>
-      <c r="H25" s="214"/>
-      <c r="I25" s="214"/>
-      <c r="J25" s="214"/>
-      <c r="K25" s="214"/>
-      <c r="L25" s="214"/>
-      <c r="M25" s="214"/>
-      <c r="N25" s="214"/>
-      <c r="O25" s="214"/>
-      <c r="P25" s="214"/>
-      <c r="Q25" s="214"/>
-      <c r="R25" s="214"/>
-      <c r="S25" s="214"/>
-      <c r="T25" s="214"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="214"/>
-      <c r="W25" s="214"/>
-      <c r="X25" s="214"/>
-      <c r="Y25" s="215"/>
+      <c r="C25" s="218"/>
+      <c r="D25" s="218"/>
+      <c r="E25" s="218"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="218"/>
+      <c r="H25" s="218"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="218"/>
+      <c r="L25" s="218"/>
+      <c r="M25" s="218"/>
+      <c r="N25" s="218"/>
+      <c r="O25" s="218"/>
+      <c r="P25" s="218"/>
+      <c r="Q25" s="218"/>
+      <c r="R25" s="218"/>
+      <c r="S25" s="218"/>
+      <c r="T25" s="218"/>
+      <c r="U25" s="218"/>
+      <c r="V25" s="218"/>
+      <c r="W25" s="218"/>
+      <c r="X25" s="218"/>
+      <c r="Y25" s="223"/>
     </row>
     <row r="26" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="141" t="s">
@@ -6979,7 +6979,7 @@
       <c r="B35" s="208"/>
       <c r="C35" s="209"/>
       <c r="D35" s="209"/>
-      <c r="E35" s="220"/>
+      <c r="E35" s="221"/>
       <c r="F35" s="209"/>
       <c r="G35" s="209"/>
       <c r="H35" s="209"/>
@@ -6988,16 +6988,16 @@
       <c r="K35" s="209"/>
       <c r="L35" s="209"/>
       <c r="M35" s="209"/>
-      <c r="N35" s="220"/>
-      <c r="O35" s="220"/>
-      <c r="P35" s="220"/>
-      <c r="Q35" s="220"/>
-      <c r="R35" s="220"/>
-      <c r="S35" s="220"/>
-      <c r="T35" s="220"/>
-      <c r="U35" s="220"/>
-      <c r="V35" s="220"/>
-      <c r="W35" s="220"/>
+      <c r="N35" s="221"/>
+      <c r="O35" s="221"/>
+      <c r="P35" s="221"/>
+      <c r="Q35" s="221"/>
+      <c r="R35" s="221"/>
+      <c r="S35" s="221"/>
+      <c r="T35" s="221"/>
+      <c r="U35" s="221"/>
+      <c r="V35" s="221"/>
+      <c r="W35" s="221"/>
       <c r="X35" s="209"/>
       <c r="Y35" s="209"/>
     </row>
@@ -7005,7 +7005,7 @@
       <c r="B36" s="209"/>
       <c r="C36" s="209"/>
       <c r="D36" s="209"/>
-      <c r="E36" s="220"/>
+      <c r="E36" s="221"/>
       <c r="F36" s="209"/>
       <c r="G36" s="209"/>
       <c r="H36" s="209"/>
@@ -7014,16 +7014,16 @@
       <c r="K36" s="209"/>
       <c r="L36" s="209"/>
       <c r="M36" s="209"/>
-      <c r="N36" s="220"/>
-      <c r="O36" s="220"/>
-      <c r="P36" s="220"/>
-      <c r="Q36" s="220"/>
-      <c r="R36" s="220"/>
-      <c r="S36" s="220"/>
-      <c r="T36" s="220"/>
-      <c r="U36" s="220"/>
-      <c r="V36" s="220"/>
-      <c r="W36" s="220"/>
+      <c r="N36" s="221"/>
+      <c r="O36" s="221"/>
+      <c r="P36" s="221"/>
+      <c r="Q36" s="221"/>
+      <c r="R36" s="221"/>
+      <c r="S36" s="221"/>
+      <c r="T36" s="221"/>
+      <c r="U36" s="221"/>
+      <c r="V36" s="221"/>
+      <c r="W36" s="221"/>
       <c r="X36" s="209"/>
       <c r="Y36" s="209"/>
     </row>
@@ -7031,7 +7031,7 @@
       <c r="B37" s="204"/>
       <c r="C37" s="204"/>
       <c r="D37" s="204"/>
-      <c r="E37" s="220"/>
+      <c r="E37" s="221"/>
       <c r="F37" s="204"/>
       <c r="G37" s="204"/>
       <c r="H37" s="204"/>
@@ -7040,16 +7040,16 @@
       <c r="K37" s="204"/>
       <c r="L37" s="204"/>
       <c r="M37" s="204"/>
-      <c r="N37" s="220"/>
-      <c r="O37" s="220"/>
-      <c r="P37" s="220"/>
-      <c r="Q37" s="220"/>
-      <c r="R37" s="220"/>
-      <c r="S37" s="220"/>
-      <c r="T37" s="220"/>
-      <c r="U37" s="220"/>
-      <c r="V37" s="220"/>
-      <c r="W37" s="220"/>
+      <c r="N37" s="221"/>
+      <c r="O37" s="221"/>
+      <c r="P37" s="221"/>
+      <c r="Q37" s="221"/>
+      <c r="R37" s="221"/>
+      <c r="S37" s="221"/>
+      <c r="T37" s="221"/>
+      <c r="U37" s="221"/>
+      <c r="V37" s="221"/>
+      <c r="W37" s="221"/>
       <c r="X37" s="204"/>
       <c r="Y37" s="204"/>
     </row>
@@ -7082,13 +7082,12 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="21">
-    <mergeCell ref="B31:Y31"/>
-    <mergeCell ref="B30:Y30"/>
-    <mergeCell ref="B35:Y35"/>
-    <mergeCell ref="B36:Y36"/>
-    <mergeCell ref="B37:Y37"/>
-    <mergeCell ref="B32:Y32"/>
-    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B25:Y25"/>
     <mergeCell ref="B2:Y2"/>
     <mergeCell ref="B4:Y4"/>
     <mergeCell ref="B11:Y11"/>
@@ -7097,12 +7096,13 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B25:Y25"/>
+    <mergeCell ref="B31:Y31"/>
+    <mergeCell ref="B30:Y30"/>
+    <mergeCell ref="B35:Y35"/>
+    <mergeCell ref="B36:Y36"/>
+    <mergeCell ref="B37:Y37"/>
+    <mergeCell ref="B32:Y32"/>
+    <mergeCell ref="B33:Y33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7269,32 +7269,32 @@
       <c r="Y3" s="206"/>
     </row>
     <row r="4" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="222" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="214"/>
-      <c r="M4" s="214"/>
-      <c r="N4" s="214"/>
-      <c r="O4" s="214"/>
-      <c r="P4" s="214"/>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="214"/>
-      <c r="S4" s="214"/>
-      <c r="T4" s="214"/>
-      <c r="U4" s="214"/>
-      <c r="V4" s="214"/>
-      <c r="W4" s="214"/>
-      <c r="X4" s="214"/>
-      <c r="Y4" s="215"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="218"/>
+      <c r="K4" s="218"/>
+      <c r="L4" s="218"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="218"/>
+      <c r="Q4" s="218"/>
+      <c r="R4" s="218"/>
+      <c r="S4" s="218"/>
+      <c r="T4" s="218"/>
+      <c r="U4" s="218"/>
+      <c r="V4" s="218"/>
+      <c r="W4" s="218"/>
+      <c r="X4" s="218"/>
+      <c r="Y4" s="223"/>
     </row>
     <row r="5" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -7507,32 +7507,32 @@
       <c r="Y10" s="135"/>
     </row>
     <row r="11" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="222" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="214"/>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="214"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="214"/>
-      <c r="M11" s="214"/>
-      <c r="N11" s="214"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="214"/>
-      <c r="Q11" s="214"/>
-      <c r="R11" s="214"/>
-      <c r="S11" s="214"/>
-      <c r="T11" s="214"/>
-      <c r="U11" s="214"/>
-      <c r="V11" s="214"/>
-      <c r="W11" s="214"/>
-      <c r="X11" s="214"/>
-      <c r="Y11" s="215"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="218"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="218"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="218"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="218"/>
+      <c r="U11" s="218"/>
+      <c r="V11" s="218"/>
+      <c r="W11" s="218"/>
+      <c r="X11" s="218"/>
+      <c r="Y11" s="223"/>
     </row>
     <row r="12" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
@@ -7745,32 +7745,32 @@
       <c r="Y17" s="135"/>
     </row>
     <row r="18" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="213" t="s">
+      <c r="B18" s="222" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="214"/>
-      <c r="O18" s="214"/>
-      <c r="P18" s="214"/>
-      <c r="Q18" s="214"/>
-      <c r="R18" s="214"/>
-      <c r="S18" s="214"/>
-      <c r="T18" s="214"/>
-      <c r="U18" s="214"/>
-      <c r="V18" s="214"/>
-      <c r="W18" s="214"/>
-      <c r="X18" s="214"/>
-      <c r="Y18" s="215"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="218"/>
+      <c r="E18" s="218"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="218"/>
+      <c r="M18" s="218"/>
+      <c r="N18" s="218"/>
+      <c r="O18" s="218"/>
+      <c r="P18" s="218"/>
+      <c r="Q18" s="218"/>
+      <c r="R18" s="218"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
+      <c r="V18" s="218"/>
+      <c r="W18" s="218"/>
+      <c r="X18" s="218"/>
+      <c r="Y18" s="223"/>
     </row>
     <row r="19" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
@@ -7983,32 +7983,32 @@
       <c r="Y24" s="137"/>
     </row>
     <row r="25" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="213" t="s">
+      <c r="B25" s="222" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="214"/>
-      <c r="D25" s="214"/>
-      <c r="E25" s="214"/>
-      <c r="F25" s="214"/>
-      <c r="G25" s="214"/>
-      <c r="H25" s="214"/>
-      <c r="I25" s="214"/>
-      <c r="J25" s="214"/>
-      <c r="K25" s="214"/>
-      <c r="L25" s="214"/>
-      <c r="M25" s="214"/>
-      <c r="N25" s="214"/>
-      <c r="O25" s="214"/>
-      <c r="P25" s="214"/>
-      <c r="Q25" s="214"/>
-      <c r="R25" s="214"/>
-      <c r="S25" s="214"/>
-      <c r="T25" s="214"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="214"/>
-      <c r="W25" s="214"/>
-      <c r="X25" s="214"/>
-      <c r="Y25" s="215"/>
+      <c r="C25" s="218"/>
+      <c r="D25" s="218"/>
+      <c r="E25" s="218"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="218"/>
+      <c r="H25" s="218"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="218"/>
+      <c r="L25" s="218"/>
+      <c r="M25" s="218"/>
+      <c r="N25" s="218"/>
+      <c r="O25" s="218"/>
+      <c r="P25" s="218"/>
+      <c r="Q25" s="218"/>
+      <c r="R25" s="218"/>
+      <c r="S25" s="218"/>
+      <c r="T25" s="218"/>
+      <c r="U25" s="218"/>
+      <c r="V25" s="218"/>
+      <c r="W25" s="218"/>
+      <c r="X25" s="218"/>
+      <c r="Y25" s="223"/>
     </row>
     <row r="26" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="141" t="s">
@@ -11341,11 +11341,11 @@
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="18">
-    <mergeCell ref="B33:Y33"/>
-    <mergeCell ref="B32:Y32"/>
-    <mergeCell ref="B31:Y31"/>
-    <mergeCell ref="B30:Y30"/>
-    <mergeCell ref="B25:Y25"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B3:Y3"/>
     <mergeCell ref="B2:Y2"/>
     <mergeCell ref="B4:Y4"/>
     <mergeCell ref="B11:Y11"/>
@@ -11354,11 +11354,11 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="B32:Y32"/>
+    <mergeCell ref="B31:Y31"/>
+    <mergeCell ref="B30:Y30"/>
+    <mergeCell ref="B25:Y25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11860,16 +11860,16 @@
       <c r="K14" s="209"/>
       <c r="L14" s="209"/>
       <c r="M14" s="209"/>
-      <c r="N14" s="220"/>
-      <c r="O14" s="220"/>
-      <c r="P14" s="220"/>
-      <c r="Q14" s="220"/>
-      <c r="R14" s="220"/>
-      <c r="S14" s="220"/>
-      <c r="T14" s="220"/>
-      <c r="U14" s="220"/>
-      <c r="V14" s="220"/>
-      <c r="W14" s="220"/>
+      <c r="N14" s="221"/>
+      <c r="O14" s="221"/>
+      <c r="P14" s="221"/>
+      <c r="Q14" s="221"/>
+      <c r="R14" s="221"/>
+      <c r="S14" s="221"/>
+      <c r="T14" s="221"/>
+      <c r="U14" s="221"/>
+      <c r="V14" s="221"/>
+      <c r="W14" s="221"/>
       <c r="X14" s="209"/>
       <c r="Y14" s="209"/>
     </row>
@@ -11886,16 +11886,16 @@
       <c r="K15" s="209"/>
       <c r="L15" s="209"/>
       <c r="M15" s="209"/>
-      <c r="N15" s="220"/>
-      <c r="O15" s="220"/>
-      <c r="P15" s="220"/>
-      <c r="Q15" s="220"/>
-      <c r="R15" s="220"/>
-      <c r="S15" s="220"/>
-      <c r="T15" s="220"/>
-      <c r="U15" s="220"/>
-      <c r="V15" s="220"/>
-      <c r="W15" s="220"/>
+      <c r="N15" s="221"/>
+      <c r="O15" s="221"/>
+      <c r="P15" s="221"/>
+      <c r="Q15" s="221"/>
+      <c r="R15" s="221"/>
+      <c r="S15" s="221"/>
+      <c r="T15" s="221"/>
+      <c r="U15" s="221"/>
+      <c r="V15" s="221"/>
+      <c r="W15" s="221"/>
       <c r="X15" s="209"/>
       <c r="Y15" s="209"/>
     </row>
@@ -11912,16 +11912,16 @@
       <c r="K16" s="204"/>
       <c r="L16" s="204"/>
       <c r="M16" s="204"/>
-      <c r="N16" s="220"/>
-      <c r="O16" s="220"/>
-      <c r="P16" s="220"/>
-      <c r="Q16" s="220"/>
-      <c r="R16" s="220"/>
-      <c r="S16" s="220"/>
-      <c r="T16" s="220"/>
-      <c r="U16" s="220"/>
-      <c r="V16" s="220"/>
-      <c r="W16" s="220"/>
+      <c r="N16" s="221"/>
+      <c r="O16" s="221"/>
+      <c r="P16" s="221"/>
+      <c r="Q16" s="221"/>
+      <c r="R16" s="221"/>
+      <c r="S16" s="221"/>
+      <c r="T16" s="221"/>
+      <c r="U16" s="221"/>
+      <c r="V16" s="221"/>
+      <c r="W16" s="221"/>
       <c r="X16" s="204"/>
       <c r="Y16" s="204"/>
     </row>
@@ -14908,32 +14908,32 @@
       <c r="Y3" s="206"/>
     </row>
     <row r="4" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="214"/>
-      <c r="M4" s="214"/>
-      <c r="N4" s="214"/>
-      <c r="O4" s="214"/>
-      <c r="P4" s="214"/>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="214"/>
-      <c r="S4" s="214"/>
-      <c r="T4" s="214"/>
-      <c r="U4" s="214"/>
-      <c r="V4" s="214"/>
-      <c r="W4" s="214"/>
-      <c r="X4" s="214"/>
-      <c r="Y4" s="215"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="218"/>
+      <c r="K4" s="218"/>
+      <c r="L4" s="218"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="218"/>
+      <c r="Q4" s="218"/>
+      <c r="R4" s="218"/>
+      <c r="S4" s="218"/>
+      <c r="T4" s="218"/>
+      <c r="U4" s="218"/>
+      <c r="V4" s="218"/>
+      <c r="W4" s="218"/>
+      <c r="X4" s="218"/>
+      <c r="Y4" s="223"/>
     </row>
     <row r="5" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="141" t="s">
@@ -15146,32 +15146,32 @@
       <c r="Y10" s="135"/>
     </row>
     <row r="11" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="222" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="214"/>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="214"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="214"/>
-      <c r="M11" s="214"/>
-      <c r="N11" s="214"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="214"/>
-      <c r="Q11" s="214"/>
-      <c r="R11" s="214"/>
-      <c r="S11" s="214"/>
-      <c r="T11" s="214"/>
-      <c r="U11" s="214"/>
-      <c r="V11" s="214"/>
-      <c r="W11" s="214"/>
-      <c r="X11" s="214"/>
-      <c r="Y11" s="215"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="218"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="218"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="218"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="218"/>
+      <c r="U11" s="218"/>
+      <c r="V11" s="218"/>
+      <c r="W11" s="218"/>
+      <c r="X11" s="218"/>
+      <c r="Y11" s="223"/>
     </row>
     <row r="12" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
@@ -15384,32 +15384,32 @@
       <c r="Y17" s="159"/>
     </row>
     <row r="18" spans="2:26" s="110" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="213" t="s">
+      <c r="B18" s="222" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="214"/>
-      <c r="O18" s="214"/>
-      <c r="P18" s="214"/>
-      <c r="Q18" s="214"/>
-      <c r="R18" s="214"/>
-      <c r="S18" s="214"/>
-      <c r="T18" s="214"/>
-      <c r="U18" s="214"/>
-      <c r="V18" s="214"/>
-      <c r="W18" s="214"/>
-      <c r="X18" s="214"/>
-      <c r="Y18" s="215"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="218"/>
+      <c r="E18" s="218"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="218"/>
+      <c r="M18" s="218"/>
+      <c r="N18" s="218"/>
+      <c r="O18" s="218"/>
+      <c r="P18" s="218"/>
+      <c r="Q18" s="218"/>
+      <c r="R18" s="218"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
+      <c r="V18" s="218"/>
+      <c r="W18" s="218"/>
+      <c r="X18" s="218"/>
+      <c r="Y18" s="223"/>
     </row>
     <row r="19" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
@@ -15570,30 +15570,30 @@
       <c r="Z22" s="125"/>
     </row>
     <row r="23" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="229"/>
-      <c r="C23" s="229"/>
-      <c r="D23" s="229"/>
-      <c r="E23" s="229"/>
-      <c r="F23" s="229"/>
-      <c r="G23" s="229"/>
-      <c r="H23" s="229"/>
-      <c r="I23" s="229"/>
-      <c r="J23" s="229"/>
-      <c r="K23" s="229"/>
-      <c r="L23" s="229"/>
-      <c r="M23" s="229"/>
-      <c r="N23" s="229"/>
-      <c r="O23" s="229"/>
-      <c r="P23" s="229"/>
-      <c r="Q23" s="229"/>
-      <c r="R23" s="229"/>
-      <c r="S23" s="229"/>
-      <c r="T23" s="229"/>
-      <c r="U23" s="229"/>
-      <c r="V23" s="229"/>
-      <c r="W23" s="229"/>
-      <c r="X23" s="229"/>
-      <c r="Y23" s="229"/>
+      <c r="B23" s="225"/>
+      <c r="C23" s="225"/>
+      <c r="D23" s="225"/>
+      <c r="E23" s="225"/>
+      <c r="F23" s="225"/>
+      <c r="G23" s="225"/>
+      <c r="H23" s="225"/>
+      <c r="I23" s="225"/>
+      <c r="J23" s="225"/>
+      <c r="K23" s="225"/>
+      <c r="L23" s="225"/>
+      <c r="M23" s="225"/>
+      <c r="N23" s="225"/>
+      <c r="O23" s="225"/>
+      <c r="P23" s="225"/>
+      <c r="Q23" s="225"/>
+      <c r="R23" s="225"/>
+      <c r="S23" s="225"/>
+      <c r="T23" s="225"/>
+      <c r="U23" s="225"/>
+      <c r="V23" s="225"/>
+      <c r="W23" s="225"/>
+      <c r="X23" s="225"/>
+      <c r="Y23" s="225"/>
     </row>
     <row r="24" spans="2:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="208" t="s">
@@ -18471,112 +18471,121 @@
       <c r="X956" s="108"/>
     </row>
     <row r="957" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B957" s="226"/>
-      <c r="C957" s="226"/>
-      <c r="D957" s="226"/>
-      <c r="E957" s="226"/>
-      <c r="F957" s="226"/>
-      <c r="G957" s="226"/>
-      <c r="H957" s="226"/>
-      <c r="I957" s="226"/>
-      <c r="J957" s="226"/>
-      <c r="K957" s="226"/>
-      <c r="L957" s="226"/>
-      <c r="M957" s="226"/>
-      <c r="N957" s="226"/>
-      <c r="O957" s="226"/>
-      <c r="P957" s="226"/>
-      <c r="Q957" s="226"/>
-      <c r="R957" s="226"/>
-      <c r="S957" s="226"/>
-      <c r="T957" s="226"/>
-      <c r="U957" s="226"/>
-      <c r="V957" s="226"/>
-      <c r="W957" s="226"/>
-      <c r="X957" s="226"/>
-      <c r="Y957" s="226"/>
+      <c r="B957" s="227"/>
+      <c r="C957" s="227"/>
+      <c r="D957" s="227"/>
+      <c r="E957" s="227"/>
+      <c r="F957" s="227"/>
+      <c r="G957" s="227"/>
+      <c r="H957" s="227"/>
+      <c r="I957" s="227"/>
+      <c r="J957" s="227"/>
+      <c r="K957" s="227"/>
+      <c r="L957" s="227"/>
+      <c r="M957" s="227"/>
+      <c r="N957" s="227"/>
+      <c r="O957" s="227"/>
+      <c r="P957" s="227"/>
+      <c r="Q957" s="227"/>
+      <c r="R957" s="227"/>
+      <c r="S957" s="227"/>
+      <c r="T957" s="227"/>
+      <c r="U957" s="227"/>
+      <c r="V957" s="227"/>
+      <c r="W957" s="227"/>
+      <c r="X957" s="227"/>
+      <c r="Y957" s="227"/>
     </row>
     <row r="958" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B958" s="227"/>
-      <c r="C958" s="227"/>
-      <c r="D958" s="227"/>
-      <c r="E958" s="227"/>
-      <c r="F958" s="227"/>
-      <c r="G958" s="227"/>
-      <c r="H958" s="227"/>
-      <c r="I958" s="227"/>
-      <c r="J958" s="227"/>
-      <c r="K958" s="227"/>
-      <c r="L958" s="227"/>
-      <c r="M958" s="227"/>
-      <c r="N958" s="227"/>
-      <c r="O958" s="227"/>
-      <c r="P958" s="227"/>
-      <c r="Q958" s="227"/>
-      <c r="R958" s="227"/>
-      <c r="S958" s="227"/>
-      <c r="T958" s="227"/>
-      <c r="U958" s="227"/>
-      <c r="V958" s="227"/>
-      <c r="W958" s="227"/>
-      <c r="X958" s="227"/>
-      <c r="Y958" s="227"/>
+      <c r="B958" s="228"/>
+      <c r="C958" s="228"/>
+      <c r="D958" s="228"/>
+      <c r="E958" s="228"/>
+      <c r="F958" s="228"/>
+      <c r="G958" s="228"/>
+      <c r="H958" s="228"/>
+      <c r="I958" s="228"/>
+      <c r="J958" s="228"/>
+      <c r="K958" s="228"/>
+      <c r="L958" s="228"/>
+      <c r="M958" s="228"/>
+      <c r="N958" s="228"/>
+      <c r="O958" s="228"/>
+      <c r="P958" s="228"/>
+      <c r="Q958" s="228"/>
+      <c r="R958" s="228"/>
+      <c r="S958" s="228"/>
+      <c r="T958" s="228"/>
+      <c r="U958" s="228"/>
+      <c r="V958" s="228"/>
+      <c r="W958" s="228"/>
+      <c r="X958" s="228"/>
+      <c r="Y958" s="228"/>
     </row>
     <row r="959" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B959" s="228"/>
-      <c r="C959" s="228"/>
-      <c r="D959" s="228"/>
-      <c r="E959" s="228"/>
-      <c r="F959" s="228"/>
-      <c r="G959" s="228"/>
-      <c r="H959" s="228"/>
-      <c r="I959" s="228"/>
-      <c r="J959" s="228"/>
-      <c r="K959" s="228"/>
-      <c r="L959" s="228"/>
-      <c r="M959" s="228"/>
-      <c r="N959" s="228"/>
-      <c r="O959" s="228"/>
-      <c r="P959" s="228"/>
-      <c r="Q959" s="228"/>
-      <c r="R959" s="228"/>
-      <c r="S959" s="228"/>
-      <c r="T959" s="228"/>
-      <c r="U959" s="228"/>
-      <c r="V959" s="228"/>
-      <c r="W959" s="228"/>
-      <c r="X959" s="228"/>
-      <c r="Y959" s="228"/>
+      <c r="B959" s="229"/>
+      <c r="C959" s="229"/>
+      <c r="D959" s="229"/>
+      <c r="E959" s="229"/>
+      <c r="F959" s="229"/>
+      <c r="G959" s="229"/>
+      <c r="H959" s="229"/>
+      <c r="I959" s="229"/>
+      <c r="J959" s="229"/>
+      <c r="K959" s="229"/>
+      <c r="L959" s="229"/>
+      <c r="M959" s="229"/>
+      <c r="N959" s="229"/>
+      <c r="O959" s="229"/>
+      <c r="P959" s="229"/>
+      <c r="Q959" s="229"/>
+      <c r="R959" s="229"/>
+      <c r="S959" s="229"/>
+      <c r="T959" s="229"/>
+      <c r="U959" s="229"/>
+      <c r="V959" s="229"/>
+      <c r="W959" s="229"/>
+      <c r="X959" s="229"/>
+      <c r="Y959" s="229"/>
     </row>
     <row r="960" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B960" s="225"/>
-      <c r="C960" s="225"/>
-      <c r="D960" s="225"/>
-      <c r="E960" s="225"/>
-      <c r="F960" s="225"/>
-      <c r="G960" s="225"/>
-      <c r="H960" s="225"/>
-      <c r="I960" s="225"/>
-      <c r="J960" s="225"/>
-      <c r="K960" s="225"/>
-      <c r="L960" s="225"/>
-      <c r="M960" s="225"/>
-      <c r="N960" s="225"/>
-      <c r="O960" s="225"/>
-      <c r="P960" s="225"/>
-      <c r="Q960" s="225"/>
-      <c r="R960" s="225"/>
-      <c r="S960" s="225"/>
-      <c r="T960" s="225"/>
-      <c r="U960" s="225"/>
-      <c r="V960" s="225"/>
-      <c r="W960" s="225"/>
-      <c r="X960" s="225"/>
-      <c r="Y960" s="225"/>
+      <c r="B960" s="226"/>
+      <c r="C960" s="226"/>
+      <c r="D960" s="226"/>
+      <c r="E960" s="226"/>
+      <c r="F960" s="226"/>
+      <c r="G960" s="226"/>
+      <c r="H960" s="226"/>
+      <c r="I960" s="226"/>
+      <c r="J960" s="226"/>
+      <c r="K960" s="226"/>
+      <c r="L960" s="226"/>
+      <c r="M960" s="226"/>
+      <c r="N960" s="226"/>
+      <c r="O960" s="226"/>
+      <c r="P960" s="226"/>
+      <c r="Q960" s="226"/>
+      <c r="R960" s="226"/>
+      <c r="S960" s="226"/>
+      <c r="T960" s="226"/>
+      <c r="U960" s="226"/>
+      <c r="V960" s="226"/>
+      <c r="W960" s="226"/>
+      <c r="X960" s="226"/>
+      <c r="Y960" s="226"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="19">
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B960:Y960"/>
+    <mergeCell ref="B957:Y957"/>
+    <mergeCell ref="B958:Y958"/>
+    <mergeCell ref="B25:Y25"/>
+    <mergeCell ref="B24:Y24"/>
+    <mergeCell ref="B26:Y26"/>
+    <mergeCell ref="B959:Y959"/>
     <mergeCell ref="B23:Y23"/>
     <mergeCell ref="B18:Y18"/>
     <mergeCell ref="B11:Y11"/>
@@ -18584,18 +18593,9 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B960:Y960"/>
-    <mergeCell ref="B957:Y957"/>
-    <mergeCell ref="B958:Y958"/>
-    <mergeCell ref="B25:Y25"/>
-    <mergeCell ref="B24:Y24"/>
-    <mergeCell ref="B26:Y26"/>
-    <mergeCell ref="B959:Y959"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="B3:Y3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36706,13 +36706,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId2"/>
@@ -36724,13 +36724,13 @@
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId5"/>

</xml_diff>